<commit_message>
Updated for compatibility with MIA v1.5.1
</commit_message>
<xml_diff>
--- a/Ex3_Skeletonisation/ExampleResults/Ex3_Skeletonisation.xlsx
+++ b/Ex3_Skeletonisation/ExampleResults/Ex3_Skeletonisation.xlsx
@@ -392,7 +392,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -414,13 +414,13 @@
         <v>147.0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.3127563876249338</v>
+        <v>0.31275638762493385</v>
       </c>
       <c r="J2" t="n">
-        <v>0.3283075256047774</v>
+        <v>0.32830752560477755</v>
       </c>
       <c r="K2" t="n">
-        <v>45.975188980865255</v>
+        <v>45.975188980865234</v>
       </c>
       <c r="L2" t="n">
         <v>64.0</v>
@@ -489,7 +489,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -507,7 +507,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -525,7 +525,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -543,7 +543,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -561,7 +561,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -579,7 +579,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -597,7 +597,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -615,7 +615,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -633,7 +633,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -651,7 +651,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -669,7 +669,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -687,7 +687,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -705,7 +705,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -723,7 +723,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -741,7 +741,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -759,7 +759,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -777,7 +777,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -795,7 +795,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -813,7 +813,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -831,7 +831,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -849,7 +849,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -867,7 +867,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -885,7 +885,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -903,7 +903,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -921,7 +921,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -939,7 +939,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -957,7 +957,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -975,7 +975,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -993,7 +993,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1029,7 +1029,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1047,7 +1047,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1065,7 +1065,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1083,7 +1083,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1119,7 +1119,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1155,7 +1155,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1220,11 +1220,11 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>53.0</v>
+        <v>26.0</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -1232,7 +1232,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0.09800326080012439</v>
+        <v>0.15575925262017415</v>
       </c>
     </row>
     <row r="3">
@@ -1246,11 +1246,11 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>26.0</v>
+        <v>63.0</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -1258,7 +1258,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.15575925262017415</v>
+        <v>0.6805055291413444</v>
       </c>
     </row>
     <row r="4">
@@ -1272,11 +1272,11 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>49.0</v>
+        <v>45.0</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -1284,7 +1284,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.41391383116064684</v>
+        <v>0.4361616299209205</v>
       </c>
     </row>
     <row r="5">
@@ -1298,11 +1298,11 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>27.0</v>
+        <v>45.0</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -1310,7 +1310,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.30160914366064684</v>
+        <v>0.23004247252054733</v>
       </c>
     </row>
     <row r="6">
@@ -1324,11 +1324,11 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>27.0</v>
+        <v>45.0</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>0.820431575281444</v>
+        <v>0.4637508952523311</v>
       </c>
     </row>
     <row r="7">
@@ -1350,19 +1350,19 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>51.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F7" t="n">
-        <v>0.08335482330012439</v>
+        <v>0.41391383116064684</v>
       </c>
     </row>
     <row r="8">
@@ -1376,19 +1376,19 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>51.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>53.0</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F8" t="n">
-        <v>0.35566709196077123</v>
+        <v>0.09800326080012439</v>
       </c>
     </row>
     <row r="9">
@@ -1402,19 +1402,19 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>51.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>72.0</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F9" t="n">
-        <v>0.07561172546014927</v>
+        <v>0.7867426351612699</v>
       </c>
     </row>
     <row r="10">
@@ -1428,19 +1428,19 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>51.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>72.0</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F10" t="n">
-        <v>0.17159245910024878</v>
+        <v>0.325532458780821</v>
       </c>
     </row>
     <row r="11">
@@ -1454,19 +1454,19 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>51.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>86.0</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F11" t="n">
-        <v>0.020716018980074635</v>
+        <v>0.23980809752054733</v>
       </c>
     </row>
     <row r="12">
@@ -1480,7 +1480,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1489,10 +1489,10 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>51.0</v>
+        <v>70.0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.1256246194402239</v>
+        <v>0.08621510864009951</v>
       </c>
     </row>
     <row r="13">
@@ -1506,7 +1506,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1515,10 +1515,10 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>51.0</v>
+        <v>70.0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.02155377716002488</v>
+        <v>0.04917513580012439</v>
       </c>
     </row>
     <row r="14">
@@ -1532,7 +1532,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1541,10 +1541,10 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>51.0</v>
+        <v>70.0</v>
       </c>
       <c r="F14" t="n">
-        <v>0.4097250402608956</v>
+        <v>0.1943310052403483</v>
       </c>
     </row>
     <row r="15">
@@ -1558,19 +1558,19 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>63.0</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>70.0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.6805055291413444</v>
+        <v>0.04429232330012439</v>
       </c>
     </row>
     <row r="16">
@@ -1584,19 +1584,19 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>45.0</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>70.0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.4361616299209205</v>
+        <v>0.08739987762017415</v>
       </c>
     </row>
     <row r="17">
@@ -1610,19 +1610,19 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>45.0</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>70.0</v>
       </c>
       <c r="F17" t="n">
-        <v>0.23004247252054733</v>
+        <v>0.032504171140099514</v>
       </c>
     </row>
     <row r="18">
@@ -1636,19 +1636,19 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>45.0</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>70.0</v>
       </c>
       <c r="F18" t="n">
-        <v>0.4637508952523311</v>
+        <v>0.11990404876027366</v>
       </c>
     </row>
     <row r="19">
@@ -1662,19 +1662,19 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>74.0</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>70.0</v>
       </c>
       <c r="F19" t="n">
-        <v>0.5646465347011198</v>
+        <v>0.03131940216002488</v>
       </c>
     </row>
     <row r="20">
@@ -1688,19 +1688,19 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>73.0</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>70.0</v>
       </c>
       <c r="F20" t="n">
-        <v>0.5907361135610203</v>
+        <v>0.18658790740037318</v>
       </c>
     </row>
     <row r="21">
@@ -1714,19 +1714,19 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>86.0</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>70.0</v>
       </c>
       <c r="F21" t="n">
-        <v>0.23980809752054733</v>
+        <v>0.028459116820049757</v>
       </c>
     </row>
     <row r="22">
@@ -1740,19 +1740,19 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>72.0</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>70.0</v>
       </c>
       <c r="F22" t="n">
-        <v>0.7867426351612699</v>
+        <v>0.0146484375</v>
       </c>
     </row>
     <row r="23">
@@ -1766,11 +1766,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>72.0</v>
+        <v>73.0</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1778,7 +1778,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>0.325532458780821</v>
+        <v>0.5907361135610203</v>
       </c>
     </row>
     <row r="24">
@@ -1792,11 +1792,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>95.0</v>
+        <v>74.0</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1804,7 +1804,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>0.07188158863153496</v>
+        <v>0.5646465347011198</v>
       </c>
     </row>
     <row r="25">
@@ -1818,11 +1818,11 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>95.0</v>
+        <v>84.0</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1830,7 +1830,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>0.48698018877225646</v>
+        <v>0.06954414398007464</v>
       </c>
     </row>
     <row r="26">
@@ -1844,11 +1844,11 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>95.0</v>
+        <v>84.0</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1856,7 +1856,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>0.07156667114009951</v>
+        <v>0.6816902981214188</v>
       </c>
     </row>
     <row r="27">
@@ -1870,11 +1870,11 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>79.0</v>
+        <v>84.0</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1882,7 +1882,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>1.1033472271220421</v>
+        <v>0.23137097808032342</v>
       </c>
     </row>
     <row r="28">
@@ -1896,19 +1896,19 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
-        <v>100.0</v>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>51.0</v>
       </c>
       <c r="F28" t="n">
-        <v>1.0691675396220424</v>
+        <v>0.08335482330012439</v>
       </c>
     </row>
     <row r="29">
@@ -1922,19 +1922,19 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
-        <v>110.0</v>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>51.0</v>
       </c>
       <c r="F29" t="n">
-        <v>0.6577669830012445</v>
+        <v>0.35566709196077123</v>
       </c>
     </row>
     <row r="30">
@@ -1948,19 +1948,19 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D30" t="n">
-        <v>109.0</v>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>51.0</v>
       </c>
       <c r="F30" t="n">
-        <v>0.2951945513804478</v>
+        <v>0.07561172546014927</v>
       </c>
     </row>
     <row r="31">
@@ -1974,19 +1974,19 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D31" t="n">
-        <v>109.0</v>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>51.0</v>
       </c>
       <c r="F31" t="n">
-        <v>0.5829930157210452</v>
+        <v>0.17159245910024878</v>
       </c>
     </row>
     <row r="32">
@@ -2000,19 +2000,19 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D32" t="n">
-        <v>109.0</v>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>51.0</v>
       </c>
       <c r="F32" t="n">
-        <v>0.22596532489180862</v>
+        <v>0.020716018980074635</v>
       </c>
     </row>
     <row r="33">
@@ -2026,19 +2026,19 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D33" t="n">
-        <v>113.0</v>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>51.0</v>
       </c>
       <c r="F33" t="n">
-        <v>0.9062996731214197</v>
+        <v>0.1256246194402239</v>
       </c>
     </row>
     <row r="34">
@@ -2052,19 +2052,19 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D34" t="n">
-        <v>113.0</v>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>51.0</v>
       </c>
       <c r="F34" t="n">
-        <v>0.1943310052403483</v>
+        <v>0.02155377716002488</v>
       </c>
     </row>
     <row r="35">
@@ -2078,19 +2078,19 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D35" t="n">
-        <v>121.0</v>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>51.0</v>
       </c>
       <c r="F35" t="n">
-        <v>0.27852358672042293</v>
+        <v>0.4097250402608956</v>
       </c>
     </row>
     <row r="36">
@@ -2104,19 +2104,19 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E36" t="n">
-        <v>70.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F36" t="n">
-        <v>0.08621510864009951</v>
+        <v>0.30160914366064684</v>
       </c>
     </row>
     <row r="37">
@@ -2130,19 +2130,19 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E37" t="n">
-        <v>70.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F37" t="n">
-        <v>0.04917513580012439</v>
+        <v>0.820431575281444</v>
       </c>
     </row>
     <row r="38">
@@ -2156,19 +2156,19 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E38" t="n">
-        <v>70.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>109.0</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F38" t="n">
-        <v>0.1943310052403483</v>
+        <v>0.2951945513804478</v>
       </c>
     </row>
     <row r="39">
@@ -2182,19 +2182,19 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E39" t="n">
-        <v>70.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>109.0</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F39" t="n">
-        <v>0.04429232330012439</v>
+        <v>0.5829930157210452</v>
       </c>
     </row>
     <row r="40">
@@ -2208,19 +2208,19 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E40" t="n">
-        <v>70.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>109.0</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F40" t="n">
-        <v>0.08739987762017415</v>
+        <v>0.22596532489180862</v>
       </c>
     </row>
     <row r="41">
@@ -2234,19 +2234,19 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E41" t="n">
-        <v>70.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>110.0</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F41" t="n">
-        <v>0.032504171140099514</v>
+        <v>0.6577669830012445</v>
       </c>
     </row>
     <row r="42">
@@ -2260,19 +2260,19 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E42" t="n">
-        <v>70.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>52.0</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F42" t="n">
-        <v>0.11990404876027366</v>
+        <v>1.099302172801993</v>
       </c>
     </row>
     <row r="43">
@@ -2286,19 +2286,19 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E43" t="n">
-        <v>70.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F43" t="n">
-        <v>0.03131940216002488</v>
+        <v>1.0691675396220424</v>
       </c>
     </row>
     <row r="44">
@@ -2312,19 +2312,19 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E44" t="n">
-        <v>70.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>121.0</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F44" t="n">
-        <v>0.18658790740037318</v>
+        <v>0.27852358672042293</v>
       </c>
     </row>
     <row r="45">
@@ -2338,19 +2338,19 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E45" t="n">
-        <v>70.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>79.0</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F45" t="n">
-        <v>0.028459116820049757</v>
+        <v>1.1033472271220421</v>
       </c>
     </row>
     <row r="46">
@@ -2364,19 +2364,19 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E46" t="n">
-        <v>70.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>113.0</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F46" t="n">
-        <v>0.0146484375</v>
+        <v>0.9062996731214197</v>
       </c>
     </row>
     <row r="47">
@@ -2390,19 +2390,19 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E47" t="n">
-        <v>34.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>113.0</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F47" t="n">
-        <v>0.2044436410404727</v>
+        <v>0.1943310052403483</v>
       </c>
     </row>
     <row r="48">
@@ -2416,19 +2416,19 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E48" t="n">
-        <v>34.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>115.0</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F48" t="n">
-        <v>1.0733563305217932</v>
+        <v>0.5543901623212939</v>
       </c>
     </row>
     <row r="49">
@@ -2442,19 +2442,19 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E49" t="n">
-        <v>34.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>115.0</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F49" t="n">
-        <v>0.35497307036052245</v>
+        <v>0.5216827169607712</v>
       </c>
     </row>
     <row r="50">
@@ -2468,19 +2468,19 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E50" t="n">
-        <v>34.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>122.0</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F50" t="n">
-        <v>0.2955415621805722</v>
+        <v>0.18052032592029854</v>
       </c>
     </row>
     <row r="51">
@@ -2494,19 +2494,19 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E51" t="n">
-        <v>34.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>122.0</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F51" t="n">
-        <v>0.42890927946077123</v>
+        <v>0.09514297546014927</v>
       </c>
     </row>
     <row r="52">
@@ -2520,19 +2520,19 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E52" t="n">
-        <v>34.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>122.0</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F52" t="n">
-        <v>0.1650341302403483</v>
+        <v>0.14058797443165935</v>
       </c>
     </row>
     <row r="53">
@@ -2546,7 +2546,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2555,10 +2555,10 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>34.0</v>
+        <v>151.0</v>
       </c>
       <c r="F53" t="n">
-        <v>0.403657458780821</v>
+        <v>0.025598831480074635</v>
       </c>
     </row>
     <row r="54">
@@ -2572,7 +2572,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -2581,10 +2581,10 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>34.0</v>
+        <v>151.0</v>
       </c>
       <c r="F54" t="n">
-        <v>0.30935224150062196</v>
+        <v>0.042269796140099514</v>
       </c>
     </row>
     <row r="55">
@@ -2598,7 +2598,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -2607,10 +2607,10 @@
         </is>
       </c>
       <c r="E55" t="n">
-        <v>34.0</v>
+        <v>151.0</v>
       </c>
       <c r="F55" t="n">
-        <v>0.08133229614009951</v>
+        <v>0.1353902444402239</v>
       </c>
     </row>
     <row r="56">
@@ -2624,19 +2624,19 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D56" t="n">
-        <v>122.0</v>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>151.0</v>
       </c>
       <c r="F56" t="n">
-        <v>0.18052032592029854</v>
+        <v>0.21504702422042293</v>
       </c>
     </row>
     <row r="57">
@@ -2650,11 +2650,11 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>122.0</v>
+        <v>95.0</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2662,7 +2662,7 @@
         </is>
       </c>
       <c r="F57" t="n">
-        <v>0.09514297546014927</v>
+        <v>0.07188158863153496</v>
       </c>
     </row>
     <row r="58">
@@ -2676,11 +2676,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>122.0</v>
+        <v>95.0</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -2688,7 +2688,7 @@
         </is>
       </c>
       <c r="F58" t="n">
-        <v>0.14058797443165935</v>
+        <v>0.48698018877225646</v>
       </c>
     </row>
     <row r="59">
@@ -2702,11 +2702,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>118.0</v>
+        <v>95.0</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2714,7 +2714,7 @@
         </is>
       </c>
       <c r="F59" t="n">
-        <v>0.22801994536052245</v>
+        <v>0.07156667114009951</v>
       </c>
     </row>
     <row r="60">
@@ -2728,11 +2728,11 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>118.0</v>
+        <v>143.0</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -2740,7 +2740,7 @@
         </is>
       </c>
       <c r="F60" t="n">
-        <v>0.47926918424097026</v>
+        <v>0.1455028802403483</v>
       </c>
     </row>
     <row r="61">
@@ -2754,11 +2754,11 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>118.0</v>
+        <v>143.0</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2766,7 +2766,7 @@
         </is>
       </c>
       <c r="F61" t="n">
-        <v>0.06752161682004976</v>
+        <v>0.9871412218816937</v>
       </c>
     </row>
     <row r="62">
@@ -2780,11 +2780,11 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>118.0</v>
+        <v>150.0</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2792,7 +2792,7 @@
         </is>
       </c>
       <c r="F62" t="n">
-        <v>0.2630373910404727</v>
+        <v>1.0988114254221673</v>
       </c>
     </row>
     <row r="63">
@@ -2806,11 +2806,11 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>115.0</v>
+        <v>155.0</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2818,7 +2818,7 @@
         </is>
       </c>
       <c r="F63" t="n">
-        <v>0.5543901623212939</v>
+        <v>1.0850007461021174</v>
       </c>
     </row>
     <row r="64">
@@ -2832,11 +2832,11 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>115.0</v>
+        <v>118.0</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2844,7 +2844,7 @@
         </is>
       </c>
       <c r="F64" t="n">
-        <v>0.5216827169607712</v>
+        <v>0.22801994536052245</v>
       </c>
     </row>
     <row r="65">
@@ -2858,11 +2858,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>140.0</v>
+        <v>118.0</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2870,7 +2870,7 @@
         </is>
       </c>
       <c r="F65" t="n">
-        <v>0.18540313842029854</v>
+        <v>0.47926918424097026</v>
       </c>
     </row>
     <row r="66">
@@ -2884,11 +2884,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>140.0</v>
+        <v>118.0</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2896,7 +2896,7 @@
         </is>
       </c>
       <c r="F66" t="n">
-        <v>0.08453959228019903</v>
+        <v>0.06752161682004976</v>
       </c>
     </row>
     <row r="67">
@@ -2910,11 +2910,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>140.0</v>
+        <v>118.0</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="F67" t="n">
-        <v>0.47606188810087074</v>
+        <v>0.2630373910404727</v>
       </c>
     </row>
     <row r="68">
@@ -2936,11 +2936,11 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>140.0</v>
+        <v>175.0</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2948,7 +2948,7 @@
         </is>
       </c>
       <c r="F68" t="n">
-        <v>0.27719508116064684</v>
+        <v>0.06096328796014927</v>
       </c>
     </row>
     <row r="69">
@@ -2962,11 +2962,11 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>84.0</v>
+        <v>175.0</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2974,7 +2974,7 @@
         </is>
       </c>
       <c r="F69" t="n">
-        <v>0.06954414398007464</v>
+        <v>0.07561172546014927</v>
       </c>
     </row>
     <row r="70">
@@ -2988,11 +2988,11 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>84.0</v>
+        <v>175.0</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3000,7 +3000,7 @@
         </is>
       </c>
       <c r="F70" t="n">
-        <v>0.6816902981214188</v>
+        <v>0.9797451348418431</v>
       </c>
     </row>
     <row r="71">
@@ -3014,11 +3014,11 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>84.0</v>
+        <v>175.0</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -3026,7 +3026,7 @@
         </is>
       </c>
       <c r="F71" t="n">
-        <v>0.23137097808032342</v>
+        <v>0.011788152160024878</v>
       </c>
     </row>
     <row r="72">
@@ -3040,19 +3040,19 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E72" t="n">
-        <v>151.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>198.0</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F72" t="n">
-        <v>0.025598831480074635</v>
+        <v>0.13371472808032342</v>
       </c>
     </row>
     <row r="73">
@@ -3066,19 +3066,19 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E73" t="n">
-        <v>151.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>168.0</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F73" t="n">
-        <v>0.042269796140099514</v>
+        <v>1.1277612896220428</v>
       </c>
     </row>
     <row r="74">
@@ -3092,19 +3092,19 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E74" t="n">
-        <v>151.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F74" t="n">
-        <v>0.1353902444402239</v>
+        <v>0.18540313842029854</v>
       </c>
     </row>
     <row r="75">
@@ -3118,19 +3118,19 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E75" t="n">
-        <v>151.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F75" t="n">
-        <v>0.21504702422042293</v>
+        <v>0.08453959228019903</v>
       </c>
     </row>
     <row r="76">
@@ -3144,11 +3144,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>143.0</v>
+        <v>140.0</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3156,7 +3156,7 @@
         </is>
       </c>
       <c r="F76" t="n">
-        <v>0.1455028802403483</v>
+        <v>0.47606188810087074</v>
       </c>
     </row>
     <row r="77">
@@ -3170,11 +3170,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>143.0</v>
+        <v>140.0</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -3182,7 +3182,7 @@
         </is>
       </c>
       <c r="F77" t="n">
-        <v>0.9871412218816937</v>
+        <v>0.27719508116064684</v>
       </c>
     </row>
     <row r="78">
@@ -3196,19 +3196,19 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E78" t="n">
-        <v>145.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>161.0</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F78" t="n">
-        <v>0.45199483640099514</v>
+        <v>1.0873702840622668</v>
       </c>
     </row>
     <row r="79">
@@ -3222,19 +3222,19 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E79" t="n">
-        <v>145.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>173.0</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F79" t="n">
-        <v>0.3544823229806966</v>
+        <v>0.909363232681818</v>
       </c>
     </row>
     <row r="80">
@@ -3248,19 +3248,19 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E80" t="n">
-        <v>145.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>173.0</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F80" t="n">
-        <v>0.07930976898007464</v>
+        <v>0.11348945648007464</v>
       </c>
     </row>
     <row r="81">
@@ -3274,19 +3274,19 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E81" t="n">
-        <v>145.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>132.0</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F81" t="n">
-        <v>0.08823763580012439</v>
+        <v>0.10407084228019903</v>
       </c>
     </row>
     <row r="82">
@@ -3300,11 +3300,11 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>150.0</v>
+        <v>132.0</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -3312,7 +3312,7 @@
         </is>
       </c>
       <c r="F82" t="n">
-        <v>1.0988114254221673</v>
+        <v>1.0352753252814446</v>
       </c>
     </row>
     <row r="83">
@@ -3326,11 +3326,11 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>52.0</v>
+        <v>216.0</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -3338,7 +3338,7 @@
         </is>
       </c>
       <c r="F83" t="n">
-        <v>1.099302172801993</v>
+        <v>0.028459116820049757</v>
       </c>
     </row>
     <row r="84">
@@ -3352,11 +3352,11 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>161.0</v>
+        <v>216.0</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3364,7 +3364,7 @@
         </is>
       </c>
       <c r="F84" t="n">
-        <v>1.0873702840622668</v>
+        <v>0.037386983640099514</v>
       </c>
     </row>
     <row r="85">
@@ -3378,11 +3378,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>198.0</v>
+        <v>216.0</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3390,7 +3390,7 @@
         </is>
       </c>
       <c r="F85" t="n">
-        <v>0.13371472808032342</v>
+        <v>0.023576304320049757</v>
       </c>
     </row>
     <row r="86">
@@ -3404,11 +3404,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>155.0</v>
+        <v>216.0</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3416,7 +3416,7 @@
         </is>
       </c>
       <c r="F86" t="n">
-        <v>1.0850007461021174</v>
+        <v>0.06786862762017415</v>
       </c>
     </row>
     <row r="87">
@@ -3430,11 +3430,11 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>175.0</v>
+        <v>216.0</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3442,7 +3442,7 @@
         </is>
       </c>
       <c r="F87" t="n">
-        <v>0.06096328796014927</v>
+        <v>0.023576304320049757</v>
       </c>
     </row>
     <row r="88">
@@ -3456,11 +3456,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>175.0</v>
+        <v>216.0</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -3468,7 +3468,7 @@
         </is>
       </c>
       <c r="F88" t="n">
-        <v>0.07561172546014927</v>
+        <v>0.05405794830012439</v>
       </c>
     </row>
     <row r="89">
@@ -3482,11 +3482,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>175.0</v>
+        <v>216.0</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3494,7 +3494,7 @@
         </is>
       </c>
       <c r="F89" t="n">
-        <v>0.9797451348418431</v>
+        <v>0.20528139922042293</v>
       </c>
     </row>
     <row r="90">
@@ -3508,11 +3508,11 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>175.0</v>
+        <v>216.0</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3520,7 +3520,7 @@
         </is>
       </c>
       <c r="F90" t="n">
-        <v>0.011788152160024878</v>
+        <v>0.023576304320049757</v>
       </c>
     </row>
     <row r="91">
@@ -3534,11 +3534,11 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>173.0</v>
+        <v>216.0</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3546,7 +3546,7 @@
         </is>
       </c>
       <c r="F91" t="n">
-        <v>0.909363232681818</v>
+        <v>0.0580709093114852</v>
       </c>
     </row>
     <row r="92">
@@ -3560,11 +3560,11 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>173.0</v>
+        <v>253.0</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3572,7 +3572,7 @@
         </is>
       </c>
       <c r="F92" t="n">
-        <v>0.11348945648007464</v>
+        <v>0.11383646728019903</v>
       </c>
     </row>
     <row r="93">
@@ -3586,11 +3586,11 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>216.0</v>
+        <v>279.0</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -3598,7 +3598,7 @@
         </is>
       </c>
       <c r="F93" t="n">
-        <v>0.028459116820049757</v>
+        <v>0.23053321990037318</v>
       </c>
     </row>
     <row r="94">
@@ -3612,19 +3612,19 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D94" t="n">
-        <v>216.0</v>
-      </c>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E94" t="n">
+        <v>165.0</v>
       </c>
       <c r="F94" t="n">
-        <v>0.037386983640099514</v>
+        <v>0.4560398907210449</v>
       </c>
     </row>
     <row r="95">
@@ -3638,19 +3638,19 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D95" t="n">
-        <v>216.0</v>
-      </c>
-      <c r="E95" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E95" t="n">
+        <v>165.0</v>
       </c>
       <c r="F95" t="n">
-        <v>0.023576304320049757</v>
+        <v>0.03131940216002488</v>
       </c>
     </row>
     <row r="96">
@@ -3664,19 +3664,19 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D96" t="n">
-        <v>216.0</v>
-      </c>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E96" t="n">
+        <v>165.0</v>
       </c>
       <c r="F96" t="n">
-        <v>0.06786862762017415</v>
+        <v>1.0780954064420925</v>
       </c>
     </row>
     <row r="97">
@@ -3690,19 +3690,19 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D97" t="n">
-        <v>216.0</v>
-      </c>
-      <c r="E97" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E97" t="n">
+        <v>165.0</v>
       </c>
       <c r="F97" t="n">
-        <v>0.023576304320049757</v>
+        <v>0.03822474182004976</v>
       </c>
     </row>
     <row r="98">
@@ -3716,19 +3716,19 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D98" t="n">
-        <v>216.0</v>
-      </c>
-      <c r="E98" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E98" t="n">
+        <v>165.0</v>
       </c>
       <c r="F98" t="n">
-        <v>0.05405794830012439</v>
+        <v>0.040247268980074635</v>
       </c>
     </row>
     <row r="99">
@@ -3742,19 +3742,19 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D99" t="n">
-        <v>216.0</v>
-      </c>
-      <c r="E99" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E99" t="n">
+        <v>165.0</v>
       </c>
       <c r="F99" t="n">
-        <v>0.20528139922042293</v>
+        <v>0.5557186678810699</v>
       </c>
     </row>
     <row r="100">
@@ -3768,19 +3768,19 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D100" t="n">
-        <v>216.0</v>
-      </c>
-      <c r="E100" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E100" t="n">
+        <v>181.0</v>
       </c>
       <c r="F100" t="n">
-        <v>0.023576304320049757</v>
+        <v>0.037386983640099514</v>
       </c>
     </row>
     <row r="101">
@@ -3794,19 +3794,19 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D101" t="n">
-        <v>216.0</v>
-      </c>
-      <c r="E101" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E101" t="n">
+        <v>181.0</v>
       </c>
       <c r="F101" t="n">
-        <v>0.0580709093114852</v>
+        <v>0.13455248626027366</v>
       </c>
     </row>
     <row r="102">
@@ -3820,19 +3820,19 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D102" t="n">
-        <v>132.0</v>
-      </c>
-      <c r="E102" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E102" t="n">
+        <v>181.0</v>
       </c>
       <c r="F102" t="n">
-        <v>0.10407084228019903</v>
+        <v>0.5245430023007465</v>
       </c>
     </row>
     <row r="103">
@@ -3846,19 +3846,19 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D103" t="n">
-        <v>132.0</v>
-      </c>
-      <c r="E103" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E103" t="n">
+        <v>181.0</v>
       </c>
       <c r="F103" t="n">
-        <v>1.0352753252814446</v>
+        <v>0.39758987730074635</v>
       </c>
     </row>
     <row r="104">
@@ -3872,19 +3872,19 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D104" t="n">
-        <v>253.0</v>
-      </c>
-      <c r="E104" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E104" t="n">
+        <v>181.0</v>
       </c>
       <c r="F104" t="n">
-        <v>0.11383646728019903</v>
+        <v>0.04310755432004976</v>
       </c>
     </row>
     <row r="105">
@@ -3898,7 +3898,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -3907,10 +3907,10 @@
         </is>
       </c>
       <c r="E105" t="n">
-        <v>181.0</v>
+        <v>145.0</v>
       </c>
       <c r="F105" t="n">
-        <v>0.037386983640099514</v>
+        <v>0.45199483640099514</v>
       </c>
     </row>
     <row r="106">
@@ -3924,7 +3924,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3936,7 +3936,7 @@
         <v>181.0</v>
       </c>
       <c r="F106" t="n">
-        <v>0.13455248626027366</v>
+        <v>0.018693491820049757</v>
       </c>
     </row>
     <row r="107">
@@ -3950,7 +3950,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3959,10 +3959,10 @@
         </is>
       </c>
       <c r="E107" t="n">
-        <v>181.0</v>
+        <v>145.0</v>
       </c>
       <c r="F107" t="n">
-        <v>0.5245430023007465</v>
+        <v>0.3544823229806966</v>
       </c>
     </row>
     <row r="108">
@@ -3976,7 +3976,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -3985,10 +3985,10 @@
         </is>
       </c>
       <c r="E108" t="n">
-        <v>181.0</v>
+        <v>145.0</v>
       </c>
       <c r="F108" t="n">
-        <v>0.39758987730074635</v>
+        <v>0.07930976898007464</v>
       </c>
     </row>
     <row r="109">
@@ -4002,7 +4002,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -4011,10 +4011,10 @@
         </is>
       </c>
       <c r="E109" t="n">
-        <v>181.0</v>
+        <v>145.0</v>
       </c>
       <c r="F109" t="n">
-        <v>0.04310755432004976</v>
+        <v>0.08823763580012439</v>
       </c>
     </row>
     <row r="110">
@@ -4028,19 +4028,19 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D110" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E110" t="n">
-        <v>181.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
+        <v>262.0</v>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F110" t="n">
-        <v>0.018693491820049757</v>
+        <v>1.0937253387017436</v>
       </c>
     </row>
     <row r="111">
@@ -4054,19 +4054,19 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D111" t="n">
-        <v>279.0</v>
-      </c>
-      <c r="E111" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E111" t="n">
+        <v>211.0</v>
       </c>
       <c r="F111" t="n">
-        <v>0.23053321990037318</v>
+        <v>0.39961240446077123</v>
       </c>
     </row>
     <row r="112">
@@ -4080,19 +4080,19 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D112" t="n">
-        <v>262.0</v>
-      </c>
-      <c r="E112" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E112" t="n">
+        <v>211.0</v>
       </c>
       <c r="F112" t="n">
-        <v>1.0937253387017436</v>
+        <v>0.045130081480074635</v>
       </c>
     </row>
     <row r="113">
@@ -4106,19 +4106,19 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D113" t="n">
-        <v>223.0</v>
-      </c>
-      <c r="E113" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E113" t="n">
+        <v>211.0</v>
       </c>
       <c r="F113" t="n">
-        <v>0.2333935052403483</v>
+        <v>0.2288577035404727</v>
       </c>
     </row>
     <row r="114">
@@ -4132,24 +4132,24 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D114" t="n">
-        <v>223.0</v>
-      </c>
-      <c r="E114" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E114" t="n">
+        <v>34.0</v>
       </c>
       <c r="F114" t="n">
-        <v>0.6700458825410953</v>
+        <v>0.2044436410404727</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>114.0</v>
+        <v>115.0</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
@@ -4158,24 +4158,24 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D115" t="n">
-        <v>223.0</v>
-      </c>
-      <c r="E115" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E115" t="n">
+        <v>34.0</v>
       </c>
       <c r="F115" t="n">
-        <v>0.18540313842029854</v>
+        <v>1.0733563305217932</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>115.0</v>
+        <v>114.0</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
@@ -4184,19 +4184,19 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D116" t="n">
-        <v>223.0</v>
-      </c>
-      <c r="E116" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E116" t="n">
+        <v>211.0</v>
       </c>
       <c r="F116" t="n">
-        <v>0.040247268980074635</v>
+        <v>0.34101865446077123</v>
       </c>
     </row>
     <row r="117">
@@ -4210,19 +4210,19 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D117" t="n">
-        <v>223.0</v>
-      </c>
-      <c r="E117" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E117" t="n">
+        <v>211.0</v>
       </c>
       <c r="F117" t="n">
-        <v>0.06096328796014927</v>
+        <v>0.5675068200410949</v>
       </c>
     </row>
     <row r="118">
@@ -4236,19 +4236,19 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D118" t="n">
-        <v>168.0</v>
-      </c>
-      <c r="E118" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E118" t="n">
+        <v>34.0</v>
       </c>
       <c r="F118" t="n">
-        <v>1.1277612896220428</v>
+        <v>0.35497307036052245</v>
       </c>
     </row>
     <row r="119">
@@ -4262,7 +4262,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -4271,10 +4271,10 @@
         </is>
       </c>
       <c r="E119" t="n">
-        <v>211.0</v>
+        <v>34.0</v>
       </c>
       <c r="F119" t="n">
-        <v>0.39961240446077123</v>
+        <v>0.2955415621805722</v>
       </c>
     </row>
     <row r="120">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -4297,10 +4297,10 @@
         </is>
       </c>
       <c r="E120" t="n">
-        <v>211.0</v>
+        <v>34.0</v>
       </c>
       <c r="F120" t="n">
-        <v>0.045130081480074635</v>
+        <v>0.42890927946077123</v>
       </c>
     </row>
     <row r="121">
@@ -4314,7 +4314,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -4323,10 +4323,10 @@
         </is>
       </c>
       <c r="E121" t="n">
-        <v>211.0</v>
+        <v>34.0</v>
       </c>
       <c r="F121" t="n">
-        <v>0.2288577035404727</v>
+        <v>0.1650341302403483</v>
       </c>
     </row>
     <row r="122">
@@ -4340,7 +4340,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -4349,10 +4349,10 @@
         </is>
       </c>
       <c r="E122" t="n">
-        <v>211.0</v>
+        <v>34.0</v>
       </c>
       <c r="F122" t="n">
-        <v>0.34101865446077123</v>
+        <v>0.403657458780821</v>
       </c>
     </row>
     <row r="123">
@@ -4366,7 +4366,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -4378,7 +4378,7 @@
         <v>211.0</v>
       </c>
       <c r="F123" t="n">
-        <v>0.5675068200410949</v>
+        <v>0.1012105569402239</v>
       </c>
     </row>
     <row r="124">
@@ -4392,7 +4392,7 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -4401,10 +4401,10 @@
         </is>
       </c>
       <c r="E124" t="n">
-        <v>211.0</v>
+        <v>34.0</v>
       </c>
       <c r="F124" t="n">
-        <v>0.1012105569402239</v>
+        <v>0.30935224150062196</v>
       </c>
     </row>
     <row r="125">
@@ -4418,7 +4418,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -4444,7 +4444,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -4453,10 +4453,10 @@
         </is>
       </c>
       <c r="E126" t="n">
-        <v>211.0</v>
+        <v>34.0</v>
       </c>
       <c r="F126" t="n">
-        <v>0.1995608285404727</v>
+        <v>0.08133229614009951</v>
       </c>
     </row>
     <row r="127">
@@ -4470,7 +4470,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -4482,7 +4482,7 @@
         <v>211.0</v>
       </c>
       <c r="F127" t="n">
-        <v>0.01667096466002488</v>
+        <v>0.1995608285404727</v>
       </c>
     </row>
     <row r="128">
@@ -4496,7 +4496,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -4508,7 +4508,7 @@
         <v>211.0</v>
       </c>
       <c r="F128" t="n">
-        <v>0.06298581512017415</v>
+        <v>0.01667096466002488</v>
       </c>
     </row>
     <row r="129">
@@ -4522,7 +4522,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -4534,7 +4534,7 @@
         <v>211.0</v>
       </c>
       <c r="F129" t="n">
-        <v>0.10895365478019903</v>
+        <v>0.06298581512017415</v>
       </c>
     </row>
     <row r="130">
@@ -4548,7 +4548,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -4560,7 +4560,7 @@
         <v>211.0</v>
       </c>
       <c r="F130" t="n">
-        <v>0.01667096466002488</v>
+        <v>0.10895365478019903</v>
       </c>
     </row>
     <row r="131">
@@ -4574,7 +4574,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -4583,10 +4583,10 @@
         </is>
       </c>
       <c r="E131" t="n">
-        <v>165.0</v>
+        <v>211.0</v>
       </c>
       <c r="F131" t="n">
-        <v>0.4560398907210449</v>
+        <v>0.01667096466002488</v>
       </c>
     </row>
     <row r="132">
@@ -4600,7 +4600,7 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -4609,10 +4609,10 @@
         </is>
       </c>
       <c r="E132" t="n">
-        <v>165.0</v>
+        <v>199.0</v>
       </c>
       <c r="F132" t="n">
-        <v>0.03131940216002488</v>
+        <v>0.13455248626027366</v>
       </c>
     </row>
     <row r="133">
@@ -4626,7 +4626,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -4635,10 +4635,10 @@
         </is>
       </c>
       <c r="E133" t="n">
-        <v>165.0</v>
+        <v>199.0</v>
       </c>
       <c r="F133" t="n">
-        <v>1.0780954064420925</v>
+        <v>0.050012893980074635</v>
       </c>
     </row>
     <row r="134">
@@ -4652,7 +4652,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -4661,10 +4661,10 @@
         </is>
       </c>
       <c r="E134" t="n">
-        <v>165.0</v>
+        <v>199.0</v>
       </c>
       <c r="F134" t="n">
-        <v>0.03822474182004976</v>
+        <v>0.379243396280821</v>
       </c>
     </row>
     <row r="135">
@@ -4678,19 +4678,19 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D135" t="n">
-        <v>210.0</v>
-      </c>
-      <c r="E135" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E135" t="n">
+        <v>199.0</v>
       </c>
       <c r="F135" t="n">
-        <v>1.1119280831419676</v>
+        <v>0.02643658966002488</v>
       </c>
     </row>
     <row r="136">
@@ -4704,7 +4704,7 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -4713,10 +4713,10 @@
         </is>
       </c>
       <c r="E136" t="n">
-        <v>165.0</v>
+        <v>199.0</v>
       </c>
       <c r="F136" t="n">
-        <v>0.040247268980074635</v>
+        <v>0.06668385864009951</v>
       </c>
     </row>
     <row r="137">
@@ -4730,7 +4730,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -4739,10 +4739,10 @@
         </is>
       </c>
       <c r="E137" t="n">
-        <v>165.0</v>
+        <v>199.0</v>
       </c>
       <c r="F137" t="n">
-        <v>0.5557186678810699</v>
+        <v>0.13169220092029854</v>
       </c>
     </row>
     <row r="138">
@@ -4756,7 +4756,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -4768,7 +4768,7 @@
         <v>199.0</v>
       </c>
       <c r="F138" t="n">
-        <v>0.13455248626027366</v>
+        <v>0.9440336675616439</v>
       </c>
     </row>
     <row r="139">
@@ -4782,7 +4782,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -4794,7 +4794,7 @@
         <v>199.0</v>
       </c>
       <c r="F139" t="n">
-        <v>0.050012893980074635</v>
+        <v>0.06989115478019903</v>
       </c>
     </row>
     <row r="140">
@@ -4808,7 +4808,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -4820,7 +4820,7 @@
         <v>199.0</v>
       </c>
       <c r="F140" t="n">
-        <v>0.379243396280821</v>
+        <v>0.050012893980074635</v>
       </c>
     </row>
     <row r="141">
@@ -4834,7 +4834,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -4846,7 +4846,7 @@
         <v>199.0</v>
       </c>
       <c r="F141" t="n">
-        <v>0.02643658966002488</v>
+        <v>0.8362647817615192</v>
       </c>
     </row>
     <row r="142">
@@ -4860,7 +4860,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -4872,7 +4872,7 @@
         <v>199.0</v>
       </c>
       <c r="F142" t="n">
-        <v>0.06668385864009951</v>
+        <v>0.03247207783141057</v>
       </c>
     </row>
     <row r="143">
@@ -4886,19 +4886,19 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D143" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E143" t="n">
-        <v>199.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D143" t="n">
+        <v>210.0</v>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F143" t="n">
-        <v>0.13169220092029854</v>
+        <v>1.1119280831419676</v>
       </c>
     </row>
     <row r="144">
@@ -4912,19 +4912,19 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D144" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E144" t="n">
-        <v>199.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D144" t="n">
+        <v>223.0</v>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F144" t="n">
-        <v>0.9440336675616439</v>
+        <v>0.2333935052403483</v>
       </c>
     </row>
     <row r="145">
@@ -4938,19 +4938,19 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D145" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E145" t="n">
-        <v>199.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D145" t="n">
+        <v>223.0</v>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F145" t="n">
-        <v>0.06989115478019903</v>
+        <v>0.6700458825410953</v>
       </c>
     </row>
     <row r="146">
@@ -4964,19 +4964,19 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D146" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E146" t="n">
-        <v>199.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D146" t="n">
+        <v>223.0</v>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F146" t="n">
-        <v>0.050012893980074635</v>
+        <v>0.18540313842029854</v>
       </c>
     </row>
     <row r="147">
@@ -4990,19 +4990,19 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D147" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E147" t="n">
-        <v>199.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D147" t="n">
+        <v>223.0</v>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F147" t="n">
-        <v>0.8362647817615192</v>
+        <v>0.040247268980074635</v>
       </c>
     </row>
     <row r="148">
@@ -5016,19 +5016,19 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
-        </is>
-      </c>
-      <c r="D148" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E148" t="n">
-        <v>199.0</v>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
+        </is>
+      </c>
+      <c r="D148" t="n">
+        <v>223.0</v>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F148" t="n">
-        <v>0.03247207783141057</v>
+        <v>0.06096328796014927</v>
       </c>
     </row>
   </sheetData>
@@ -5079,7 +5079,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -5097,7 +5097,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -5115,7 +5115,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -5133,7 +5133,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -5151,7 +5151,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -5169,7 +5169,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -5187,7 +5187,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -5205,7 +5205,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -5223,7 +5223,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -5239,7 +5239,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5252,96 +5252,96 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>MIA_VERSION</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1.5.1</t>
+        </is>
+      </c>
+    </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MIA_VERSION</t>
+          <t>WORKFLOW FILENAME</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1.4.2</t>
+          <t>/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/Ex3_Skeletonisation.mia</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>WORKFLOW FILENAME</t>
+          <t>OS NAME</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>F:\Java Projects\mia-examples\Ex3_Skeletonisation\Ex3_Skeletonisation.mia</t>
+          <t>Mac OS X</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>OS NAME</t>
+          <t>OS ARCHITECTURE</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Windows 10</t>
+          <t>aarch64</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>OS ARCHITECTURE</t>
+          <t>OS VERSION</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>amd64</t>
+          <t>14.3</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>OS VERSION</t>
+          <t>DATE AND TIME COMPLETED</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>10.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>DATE AND TIME COMPLETED</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2023-10-09_04-57-26</t>
+          <t>2024-02-09_10-45-51</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="16" t="inlineStr">
+        <is>
+          <t>WORKFLOW CONFIGURATION (XML)</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="16" t="inlineStr">
-        <is>
-          <t>WORKFLOW CONFIGURATION (XML)</t>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;ROOT MIA_VERSION="1.5.1"&gt;&lt;MODULES&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.core.InputControl" DISABLEABLE="false" ENABLED="true" ID="1638297565958" NAME="Input control" NICKNAME="Input control" NOTES="" SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input path" NICKNAME="Input path" VALUE="/Users/sc13967/Documents/Programming/Java/mia-examples/Ex3_Skeletonisation/Ex3_Skeletonisation.tif" VISIBLE="true"/&gt;&lt;PARAMETER NAME="Series mode" NICKNAME="Series mode" VALUE="All series" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Series list" NICKNAME="Series list" VALUE="1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Only load first file per folder" NICKNAME="Only load first file per folder" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Only load first matching group" NICKNAME="Only load first matching group" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Pattern" NICKNAME="Pattern" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Spatial unit" NICKNAME="Spatial unit" VALUE="Micrometres" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Temporal unit" NICKNAME="Temporal unit" VALUE="Milliseconds" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Ignore case" NICKNAME="Ignore case" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Add filter" NICKNAME="Add filter" VALUE="" VISIBLE="false"&gt;&lt;COLLECTION&gt;&lt;PARAMS&gt;&lt;PARAM NAME="Filter source" NICKNAME="Filter source" VALUE="Extension" VISIBLE="false"/&gt;&lt;PARAM NAME="Filter value" NICKNAME="Filter value" VALUE="tif" VISIBLE="false"/&gt;&lt;PARAM NAME="Filter type" NICKNAME="Filter type" VALUE="Matches partially (include)" VISIBLE="false"/&gt;&lt;/PARAMS&gt;&lt;PARAMS&gt;&lt;PARAM NAME="Filter source" NICKNAME="Filter source" VALUE="Filename" VISIBLE="false"/&gt;&lt;PARAM NAME="Filter value" NICKNAME="Filter value" VALUE="_overlay" VISIBLE="false"/&gt;&lt;PARAM NAME="Filter type" NICKNAME="Filter type" VALUE="Matches partially (exclude)" VISIBLE="false"/&gt;&lt;/PARAMS&gt;&lt;/COLLECTION&gt;&lt;/PARAMETER&gt;&lt;PARAMETER NAME="Simultaneous jobs" NICKNAME="Simultaneous jobs" VALUE="1" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA&gt;&lt;METADATUM EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" NAME="Extension" NICKNAME="Extension"/&gt;&lt;METADATUM EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" NAME="File" NICKNAME="File"/&gt;&lt;METADATUM EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" NAME="Filename" NICKNAME="Filename"/&gt;&lt;METADATUM EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" NAME="Filepath" NICKNAME="Filepath"/&gt;&lt;METADATUM EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" NAME="Series name" NICKNAME="Series name"/&gt;&lt;METADATUM EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" NAME="Series number" NICKNAME="Series number"/&gt;&lt;/METADATA&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.core.OutputControl" DISABLEABLE="false" ENABLED="true" ID="1638297565958" NAME="Output control" NICKNAME="Output control" NOTES="Configuring the exported Excel spreadsheet.  This will spreadsheet report the length of both the individual and network DNA ovjects. " SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Add variable" NICKNAME="Add variable" VALUE="" VISIBLE="false"&gt;&lt;COLLECTION/&gt;&lt;/PARAMETER&gt;&lt;PARAMETER NAME="Run macro" NICKNAME="Run macro" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Macro mode" NICKNAME="Macro mode" VALUE="Macro text" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Macro text" NICKNAME="Macro text" VALUE="run(&amp;quot;Enable MIA Extensions&amp;quot;);&amp;#10;&amp;#10;// Get a list of Workspace IDs with Ext.MIA_GetListOfWorkspaceIDs() and set active workspace with Ext.MIA_SetActiveWorkspace(ID)." VISIBLE="false"/&gt;&lt;PARAMETER NAME="Macro file" NICKNAME="Macro file" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Export mode" NICKNAME="Export mode" VALUE="All together" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Individual save location" NICKNAME="Individual save location" VALUE="Save with input file" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Group save location" NICKNAME="Group save location" VALUE="Save with input file" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File path" NICKNAME="File path" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Mirrored directory root" NICKNAME="Mirrored directory root" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Save name mode" NICKNAME="Save name mode" VALUE="Match input file/folder name" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File name" NICKNAME="File name" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Metadata item for grouping" NICKNAME="Metadata item for grouping" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Continuous data export" NICKNAME="Continuous data export" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Save every n files" NICKNAME="Save every n files" VALUE="10" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Append date/time mode" NICKNAME="Append date/time mode" VALUE="Never" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Export summary" NICKNAME="Export summary" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Summary mode" NICKNAME="Summary mode" VALUE="Per input file" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Metadata item for summary" NICKNAME="Metadata item for summary" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Show object counts" NICKNAME="Show object counts" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Export individual objects" NICKNAME="Export individual objects" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;/MODULES&gt;&lt;MODULES&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.system.GUISeparator" DISABLEABLE="false" ENABLED="true" ID="1694925729349" NAME="GUI separator" NICKNAME="File loading" NOTES="" SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Show in processing view" NICKNAME="Show basic" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in processing view" NICKNAME="Expanded basic GUI" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in editing view" NICKNAME="Expanded editing GUI" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.inputoutput.ImageLoader" DISABLEABLE="false" ENABLED="true" ID="1638297567118" NAME="Load image" NICKNAME="Load image" NOTES="In this standard image loading module we're loading the AFM image of DNA to the MIA workspace with the name &amp;quot;Image&amp;quot;." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="Image" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Import mode" NICKNAME="Import mode" VALUE="Current file" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reader" NICKNAME="Reader" VALUE="Bio-Formats" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Sequence root name" NICKNAME="Sequence root name" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Name format" NICKNAME="Name format" VALUE="Generic (from metadata)" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Comment" NICKNAME="Comment" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Extension" NICKNAME="Extension" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Generic format" NICKNAME="Generic format" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Include series number" NICKNAME="Include series number" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File path" NICKNAME="File path" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Series mode" NICKNAME="Series mode" VALUE="Current series" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Series number" NICKNAME="Series number" VALUE="1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Channels" NICKNAME="Channels" VALUE="1-end" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Slices" NICKNAME="Slices" VALUE="1-end" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Frames" NICKNAME="Frames" VALUE="1-end" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Channel" NICKNAME="Channel" VALUE="1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Crop mode" NICKNAME="Crop mode" VALUE="None" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference image" NICKNAME="Reference image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Left coordinate" NICKNAME="Left coordinate" VALUE="384" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Top coordinate" NICKNAME="Top coordinate" VALUE="287" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Width" NICKNAME="Width" VALUE="640" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Height" NICKNAME="Height" VALUE="640" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Objects for limits" NICKNAME="Objects for limits" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Scale mode" NICKNAME="Scale mode" VALUE="No scaling" VISIBLE="false"/&gt;&lt;PARAMETER NAME="X scale factor" NICKNAME="X scale factor" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Y scale factor" NICKNAME="Y scale factor" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Dimension mismatch mode" NICKNAME="Dimension mismatch mode" VALUE="Disallow (fail upon mismatch)" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Pad intensity mode" NICKNAME="Pad intensity mode" VALUE="Black (0)" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Set manual spatial calibration" NICKNAME="Set manual spatial calibration" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="XY calibration (dist/px)" NICKNAME="XY calibration (dist/px)" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Z calibration (dist/px)" NICKNAME="Z calibration (dist/px)" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Set manual temporal calibration" NICKNAME="Set manual temporal calibration" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Frame interval (time/frame)" NICKNAME="Frame interval (time/frame)" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Force bit depth" NICKNAME="Force bit depth" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output bit depth" NICKNAME="Output bit depth" VALUE="8" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Minimum input intensity" NICKNAME="Minimum input intensity" VALUE="0.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Maximum input intensity" NICKNAME="Maximum input intensity" VALUE="1.0" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.system.GUISeparator" DISABLEABLE="false" ENABLED="true" ID="1694925848319" NAME="GUI separator" NICKNAME="Detect DNA" NOTES="" SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Show in processing view" NICKNAME="Show basic" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in processing view" NICKNAME="Expanded basic GUI" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in editing view" NICKNAME="Expanded editing GUI" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.images.process.FilterImage" DISABLEABLE="false" ENABLED="true" ID="1694706310794" NAME="Filter image" NICKNAME="Filter image" NOTES="The first processing step is to remove some of the noise in the raw image.  To do this, we apply a 2D Gaussian filter with a sigma of 1px.  This reduces the noise, but retains the DNA features, which are of a similar width to the chosen sigma value.&amp;#10;&amp;#10;The filtered image is added to the workspace with the name &amp;quot;Filtered&amp;quot;." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Image" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Apply to input image" NICKNAME="Apply to input image" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="Filtered" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Filter mode" NICKNAME="Filter mode" VALUE="Gaussian 2D" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Filter radius" NICKNAME="Filter radius" VALUE="1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Filter radius 2" NICKNAME="Filter radius 2" VALUE="3.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Calibrated units" NICKNAME="Calibrated units" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Rolling filter method" NICKNAME="Rolling filter method" VALUE="Average" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Window indices" NICKNAME="Window indices" VALUE="-1-1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Contour contrast" NICKNAME="Contour contrast" VALUE="Dark line" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.script.RunSingleCommand" DISABLEABLE="false" ENABLED="true" ID="1638299323511" NAME="Run single command" NICKNAME="Run single command" NOTES="The mica substrate on which the DNA is deposited gives a variable background that we wish to remove prior to detection of DNA.  To achieve this, we apply rolling ball background subtraction with a ball radius of 5px.  We can use a relatively small radius as we know the DNA shouldn't be wider than approximately 2-3px.&amp;#10;&amp;#10;MIA doesn't have an explicit module to run the rolling ball subtraction.  Instead, we can run this as a single macro command using the &amp;quot;Run single command&amp;quot; module.  This module is compatible with any ImageJ commands which have a corresponding macro command in the form run(&amp;quot;[command]&amp;quot;, &amp;quot;[arguments]&amp;quot;) and which also update the input image.  To find out if a command is compatible, start ImageJ's macro recorder (Plugins &amp;gt; Macros &amp;gt; Record...) and run the operation manually from the ImageJ interface.&amp;#10;&amp;#10;Since we won't need the &amp;quot;Filtered&amp;quot; image in its original form again, we update this image in the workspace with the background-subtracted image.  This helps reduce unnecessary memory usage. " SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Filtered" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Apply to input image" NICKNAME="Apply to input image" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="Filtered" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Command" NICKNAME="Command" VALUE="Subtract Background..." VISIBLE="false"/&gt;&lt;PARAMETER NAME="Parameters" NICKNAME="Parameters" VALUE="rolling=5" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Enable multithreading" NICKNAME="Enable multithreading" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.images.process.threshold.GlobalAutoThreshold" DISABLEABLE="false" ENABLED="true" ID="1695827300950" NAME="Global auto-threshold" NICKNAME="Global auto-threshold" NOTES="The next step is to binarise the image using the &amp;quot;Global auto-threshold&amp;quot; module.  Here, we use the Otsu method and store the output in the workspace with the name &amp;quot;Binary&amp;quot;." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Filtered" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output mode" NICKNAME="Output mode" VALUE="Calculate and apply" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Apply to input image" NICKNAME="Apply to input image" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="Binary" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Algorithm" NICKNAME="Algorithm" VALUE="Otsu" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Threshold multiplier" NICKNAME="Threshold multiplier" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Use lower threshold limit" NICKNAME="Use lower threshold limit" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Lower threshold limit" NICKNAME="Lower threshold limit" VALUE="0.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Binary logic" NICKNAME="Binary logic" VALUE="Black (0) background" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure on objects" NICKNAME="Measure on objects" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" IMAGE_NAME="Binary" NAME="THRESHOLD // GLOBAL Otsu" NICKNAME="THRESHOLD // GLOBAL Otsu"/&gt;&lt;/IMAGE_MEASUREMENTS&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.detect.IdentifyObjects" DISABLEABLE="false" ENABLED="true" ID="1694706262899" NAME="Identify objects" NICKNAME="Identify objects" NOTES="The individual DNA objects are detected from the binary image using connected components labelling.  This process is done using the &amp;quot;Identify objects&amp;quot; module, which takes a binary image and identifies each connected (or 'contiguous') region as a separate object.&amp;#10;&amp;#10;These objects are added to the MIA workspace with the name DNA.&amp;#10;&amp;#10;To perform connected components labelling, MIA uses the MorphoLibJ plugin." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Binary" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output objects" NICKNAME="Output objects" VALUE="DNA" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Binary logic" NICKNAME="Binary logic" VALUE="Black (0) background" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Detection mode" NICKNAME="Detection mode" VALUE="3D" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Identify as single object" NICKNAME="Identify as single object" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Connectivity" NICKNAME="Connectivity" VALUE="26" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Volume type" NICKNAME="Volume type" VALUE="Quadtree" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Enable multithreading" NICKNAME="Enable multithreading" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Minimum strip width (px)" NICKNAME="Minimum strip width (px)" VALUE="60" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.filter.FilterOnImageEdge" DISABLEABLE="false" ENABLED="true" ID="1694706063682" NAME="Remove on image edge" NICKNAME="Remove on image edge" NOTES="One of the aims of this workflow is to measure the length of each single DNA molecule (i.e. not those where multiple molecules are overlapping).  As such, we can't accurately measure any that are in contact with the image edge.  To remove these, we use the &amp;quot;Remove on image edge&amp;quot; module.&amp;#10;&amp;#10;If we were simply counting objects, we may wish to only discard objects touching a couple of image edges (e.g. top and left); however, in this instance we want to remove DNA molecules touching any of the image edges." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="DNA" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Filter mode" NICKNAME="Filter mode" VALUE="Remove filtered objects" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output (filtered) objects" NICKNAME="Output (filtered) objects" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Maximum permitted contact" NICKNAME="Maximum permitted contact" VALUE="0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Remove on top" NICKNAME="Remove on top" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Remove on left" NICKNAME="Remove on left" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Remove on bottom" NICKNAME="Remove on bottom" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Remove on right" NICKNAME="Remove on right" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Include Z-position" NICKNAME="Include Z-position" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Store filter results" NICKNAME="Store filter results" VALUE="false" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.measure.spatial.MeasureObjectShape" DISABLEABLE="false" ENABLED="true" ID="1694998855476" NAME="Measure object shape" NICKNAME="Measure object shape" NOTES="At the moment, the &amp;quot;DNA&amp;quot; object collection contains a lot of small round objects which likely correspond to salt crystals and other debris.  To remove these, we can set a minimum diameter.&amp;#10;&amp;#10;First, we make this measurement using the &amp;quot;Measure object shape&amp;quot; module.  Measurements in 2D are calculated on Z-projected objects; however, as our objects are in 2D already this will make no difference." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="DNA" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure volume" NICKNAME="Measure volume" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure projected area" NICKNAME="Measure projected area" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure projected diameter" NICKNAME="Measure projected diameter" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure projected perimeter" NICKNAME="Measure projected perimeter" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure 3D metrics" NICKNAME="Measure 3D metrics" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Connectivity" NICKNAME="Connectivity" VALUE="26" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Surface area method" NICKNAME="Surface area method" VALUE="13 directions" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Enable multithreading" NICKNAME="Enable multithreading" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SHAPE // PROJ_DIA_(PX)" NICKNAME="SHAPE // PROJ_DIA_(PX)" OBJECT_NAME="DNA"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SHAPE // PROJ_DIA_(µm)" NICKNAME="SHAPE // PROJ_DIA_(µm)" OBJECT_NAME="DNA"/&gt;&lt;/OBJECT_MEASUREMENTS&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.filter.FilterByMeasurement" DISABLEABLE="true" ENABLED="true" ID="1694998908258" NAME="Based on measurement" NICKNAME="Based on measurement" NOTES="With the diameter measurements calculated, we can remove any &amp;quot;DNA&amp;quot; objects smaller than a specific size using the &amp;quot;Based on measurement&amp;quot; filter module." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="DNA" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Filter mode" NICKNAME="Filter mode" VALUE="Remove filtered objects" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output (filtered) objects" NICKNAME="Output (filtered) objects" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Method for filtering" NICKNAME="Method for filtering" VALUE="Less than" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference mode" NICKNAME="Reference mode" VALUE="Fixed value" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference value" NICKNAME="Reference value" VALUE="20" VISIBLE="true"/&gt;&lt;PARAMETER NAME="Reference value image" NICKNAME="Reference value image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference image measurement" NICKNAME="Reference image measurement" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference value parent object" NICKNAME="Reference value parent object" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference object measurement" NICKNAME="Reference object measurement" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference value multiplier" NICKNAME="Reference value multiplier" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Store summary filter results" NICKNAME="Store summary filter results" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Store individual filter results" NICKNAME="Store individual filter results" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measurement to filter on" NICKNAME="Measurement to filter on" VALUE="SHAPE // PROJ_DIA_(PX)" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.system.GUISeparator" DISABLEABLE="false" ENABLED="true" ID="1694925858241" NAME="GUI separator" NICKNAME="Measurements" NOTES="" SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Show in processing view" NICKNAME="Show basic" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in processing view" NICKNAME="Expanded basic GUI" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in editing view" NICKNAME="Expanded editing GUI" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.process.CreateSkeleton" DISABLEABLE="false" ENABLED="true" ID="1694925436767" NAME="Create skeleton" NICKNAME="Create skeleton" NOTES="To measure length of our &amp;quot;DNA&amp;quot; objects, we can use the &amp;quot;Measure skeleton&amp;quot; module.  Skeletonisation involves reducing objects to a single pixel-wide line.  During this process, the length of the skeleton objects is measured and added to the associated DNA object.&amp;#10;&amp;#10;Skeletons themselves are formed from networks of &amp;quot;Edges&amp;quot; and &amp;quot;Junctions&amp;quot;, where edges are line segments between two junctions.  Junctions can in turn have one or more connected edges.&amp;#10;&amp;#10;MIA provides two object relationship types, both of which are in use when creating skeletons.  Parent-child relationships allow for one-to-many relationships between objects and here, the &amp;quot;DNA&amp;quot; objects are parents to the child &amp;quot;Skeleton&amp;quot; objects.  Likewise, the &amp;quot;Edges&amp;quot; and &amp;quot;Junctions&amp;quot; are children of the &amp;quot;Skeleton&amp;quot; objects.  Since MIA allows for extended relationships, this means the &amp;quot;Edges&amp;quot; and &amp;quot;Junctions&amp;quot; are therefore grandchildren of the &amp;quot;DNA&amp;quot; objects.&amp;#10;&amp;#10;Conversely, partner relationships allow for many-to-many relationships and here are present between &amp;quot;Edges&amp;quot; and &amp;quot;Junctions&amp;quot;.&amp;#10;&amp;#10;The &amp;quot;Measure skeleton&amp;quot; module  uses the &amp;quot;Analyze Skeleton&amp;quot; ImageJ plugin." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.1.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input mode" NICKNAME="Input mode" VALUE="Objects" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Binary logic" NICKNAME="Binary logic" VALUE="Black (0) background" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="DNA" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Add skeletons to workspace" NICKNAME="Add skeletons to workspace" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output skeleton objects" NICKNAME="Output skeleton objects" VALUE="Skeletons" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output edge objects" NICKNAME="Output edge objects" VALUE="Edges" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output junction objects" NICKNAME="Output junction objects" VALUE="Junctions" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Export loop objects" NICKNAME="Export loop objects" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output loop objects" NICKNAME="Output loop objects" VALUE="Loops" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Export largest shortest path" NICKNAME="Export largest shortest path" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output largest shortest path" NICKNAME="Output largest shortest path" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Minimum branch length" NICKNAME="Minimum branch length" VALUE="5" VISIBLE="true"/&gt;&lt;PARAMETER NAME="Calibrated units" NICKNAME="Calibrated units" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Enable multithreading" NICKNAME="Enable multithreading" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SKELETON // LENGTH_(PX)" NICKNAME="SKELETON // LENGTH_(PX)" OBJECT_NAME="Edges"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" EXPORT_MAX="false" EXPORT_MEAN="true" EXPORT_MIN="false" EXPORT_STD="true" EXPORT_SUM="true" NAME="SKELETON // LENGTH_(µm)" NICKNAME="SKELETON // LENGTH_(µm)" OBJECT_NAME="Edges"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SKELETON // SUM_LENGTH_(PX)" NICKNAME="SKELETON // SUM_LENGTH_(PX)" OBJECT_NAME="DNA"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" EXPORT_MAX="false" EXPORT_MEAN="true" EXPORT_MIN="false" EXPORT_STD="true" EXPORT_SUM="true" NAME="SKELETON // SUM_LENGTH_(µm)" NICKNAME="SKELETON // SUM_LENGTH_(µm)" OBJECT_NAME="DNA"/&gt;&lt;/OBJECT_MEASUREMENTS&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.filter.FilterByPartners" DISABLEABLE="false" ENABLED="true" ID="1694706692780" NAME="Number of partners" NICKNAME="Number of partners" NOTES="For our analysis, we only want to measure the length of individual DNA molecules.  That means, we need a way of identifying any &amp;quot;DNA&amp;quot; objects formed from multiple overlapping molecules.&amp;#10;&amp;#10;One way to do this is to count the number of lose DNA ends there are, which we can do by counting the number of &amp;quot;Junction&amp;quot; objects which only have a single connected &amp;quot;Edge&amp;quot;.  For this, we use the &amp;quot;Number of partners&amp;quot; object filter.  With this filter we don't want to remove any junctions with a single connected edge; rather, we want to move them to a separate class which we call &amp;quot;Ends&amp;quot;.&amp;#10;&amp;#10;The &amp;quot;Ends&amp;quot; objects are added to the MIA workspace and automatically inherit any relationships that same object had when it was a &amp;quot;Junction&amp;quot;.  In this case these are direct relationships with &amp;quot;Skeleton&amp;quot; and &amp;quot;Edge&amp;quot; objects as well as the extended grandparent-grandchild relationship to &amp;quot;DNA&amp;quot; that arises as a result of being a child of an object (&amp;quot;Skeletons&amp;quot;) which itself is a child of a &amp;quot;DNA&amp;quot; object." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="Junctions" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Filter mode" NICKNAME="Filter mode" VALUE="Move filtered objects to new class" VISIBLE="false"/&gt;&lt;PARA</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;ROOT MIA_VERSION="1.4.2"&gt;&lt;MODULES&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.core.InputControl" DISABLEABLE="false" ENABLED="true" ID="1638297565958" NAME="Input control" NICKNAME="Input control" NOTES="" SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input path" NICKNAME="Input path" VALUE="F:\Java Projects\mia-examples\Ex3_Skeletonisation\Ex3_Skeletonisation.tif" VISIBLE="true"/&gt;&lt;PARAMETER NAME="Series mode" NICKNAME="Series mode" VALUE="All series" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Series list" NICKNAME="Series list" VALUE="1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Only load first file per folder" NICKNAME="Only load first file per folder" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Only load first matching group" NICKNAME="Only load first matching group" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Pattern" NICKNAME="Pattern" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Spatial unit" NICKNAME="Spatial unit" VALUE="Micrometres" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Temporal unit" NICKNAME="Temporal unit" VALUE="Milliseconds" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Ignore case" NICKNAME="Ignore case" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Add filter" NICKNAME="Add filter" VALUE="" VISIBLE="false"&gt;&lt;COLLECTION&gt;&lt;PARAMS&gt;&lt;PARAM NAME="Filter source" NICKNAME="Filter source" VALUE="Extension" VISIBLE="false"/&gt;&lt;PARAM NAME="Filter value" NICKNAME="Filter value" VALUE="tif" VISIBLE="false"/&gt;&lt;PARAM NAME="Filter type" NICKNAME="Filter type" VALUE="Matches partially (include)" VISIBLE="false"/&gt;&lt;/PARAMS&gt;&lt;PARAMS&gt;&lt;PARAM NAME="Filter source" NICKNAME="Filter source" VALUE="Filename" VISIBLE="false"/&gt;&lt;PARAM NAME="Filter value" NICKNAME="Filter value" VALUE="_overlay" VISIBLE="false"/&gt;&lt;PARAM NAME="Filter type" NICKNAME="Filter type" VALUE="Matches partially (exclude)" VISIBLE="false"/&gt;&lt;/PARAMS&gt;&lt;/COLLECTION&gt;&lt;/PARAMETER&gt;&lt;PARAMETER NAME="Simultaneous jobs" NICKNAME="Simultaneous jobs" VALUE="1" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA&gt;&lt;METADATUM EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" NAME="Extension" NICKNAME="Extension"/&gt;&lt;METADATUM EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" NAME="File" NICKNAME="File"/&gt;&lt;METADATUM EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" NAME="Filename" NICKNAME="Filename"/&gt;&lt;METADATUM EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" NAME="Filepath" NICKNAME="Filepath"/&gt;&lt;METADATUM EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" NAME="Series name" NICKNAME="Series name"/&gt;&lt;METADATUM EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" NAME="Series number" NICKNAME="Series number"/&gt;&lt;/METADATA&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.core.OutputControl" DISABLEABLE="false" ENABLED="true" ID="1638297565958" NAME="Output control" NICKNAME="Output control" NOTES="Configuring the exported Excel spreadsheet.  This will spreadsheet report the length of both the individual and network DNA ovjects. " SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Add variable" NICKNAME="Add variable" VALUE="" VISIBLE="false"&gt;&lt;COLLECTION/&gt;&lt;/PARAMETER&gt;&lt;PARAMETER NAME="Run macro" NICKNAME="Run macro" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Macro mode" NICKNAME="Macro mode" VALUE="Macro text" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Macro text" NICKNAME="Macro text" VALUE="run(&amp;quot;Enable MIA Extensions&amp;quot;);&amp;#10;&amp;#10;// Get a list of Workspace IDs with Ext.MIA_GetListOfWorkspaceIDs() and set active workspace with Ext.MIA_SetActiveWorkspace(ID)." VISIBLE="false"/&gt;&lt;PARAMETER NAME="Macro file" NICKNAME="Macro file" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Export mode" NICKNAME="Export mode" VALUE="All together" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Individual save location" NICKNAME="Individual save location" VALUE="Save with input file" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Group save location" NICKNAME="Group save location" VALUE="Save with input file" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File path" NICKNAME="File path" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Mirrored directory root" NICKNAME="Mirrored directory root" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Save name mode" NICKNAME="Save name mode" VALUE="Match input file/folder name" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File name" NICKNAME="File name" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Metadata item for grouping" NICKNAME="Metadata item for grouping" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Continuous data export" NICKNAME="Continuous data export" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Save every n files" NICKNAME="Save every n files" VALUE="10" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Append date/time mode" NICKNAME="Append date/time mode" VALUE="Never" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Export summary" NICKNAME="Export summary" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Summary mode" NICKNAME="Summary mode" VALUE="Per input file" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Metadata item for summary" NICKNAME="Metadata item for summary" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Show object counts" NICKNAME="Show object counts" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Export individual objects" NICKNAME="Export individual objects" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;/MODULES&gt;&lt;MODULES&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.system.GUISeparator" DISABLEABLE="false" ENABLED="true" ID="1694925729349" NAME="GUI separator" NICKNAME="File loading" NOTES="" SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Show in processing view" NICKNAME="Show basic" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in processing view" NICKNAME="Expanded basic GUI" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in editing view" NICKNAME="Expanded editing GUI" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.inputoutput.ImageLoader" DISABLEABLE="false" ENABLED="true" ID="1638297567118" NAME="Load image" NICKNAME="Load image" NOTES="In this standard image loading module we're loading the AFM image of DNA to the MIA workspace with the name &amp;quot;Image&amp;quot;." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="Image" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Import mode" NICKNAME="Import mode" VALUE="Current file" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reader" NICKNAME="Reader" VALUE="Bio-Formats" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Sequence root name" NICKNAME="Sequence root name" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Name format" NICKNAME="Name format" VALUE="Generic (from metadata)" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Comment" NICKNAME="Comment" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Extension" NICKNAME="Extension" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Generic format" NICKNAME="Generic format" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Include series number" NICKNAME="Include series number" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File path" NICKNAME="File path" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Series mode" NICKNAME="Series mode" VALUE="Current series" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Series number" NICKNAME="Series number" VALUE="1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Channels" NICKNAME="Channels" VALUE="1-end" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Slices" NICKNAME="Slices" VALUE="1-end" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Frames" NICKNAME="Frames" VALUE="1-end" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Channel" NICKNAME="Channel" VALUE="1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Crop mode" NICKNAME="Crop mode" VALUE="None" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference image" NICKNAME="Reference image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Left coordinate" NICKNAME="Left coordinate" VALUE="384" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Top coordinate" NICKNAME="Top coordinate" VALUE="287" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Width" NICKNAME="Width" VALUE="640" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Height" NICKNAME="Height" VALUE="640" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Objects for limits" NICKNAME="Objects for limits" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Scale mode" NICKNAME="Scale mode" VALUE="No scaling" VISIBLE="false"/&gt;&lt;PARAMETER NAME="X scale factor" NICKNAME="X scale factor" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Y scale factor" NICKNAME="Y scale factor" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Dimension mismatch mode" NICKNAME="Dimension mismatch mode" VALUE="Disallow (fail upon mismatch)" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Pad intensity mode" NICKNAME="Pad intensity mode" VALUE="Black (0)" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Set manual spatial calibration" NICKNAME="Set manual spatial calibration" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="XY calibration (dist/px)" NICKNAME="XY calibration (dist/px)" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Z calibration (dist/px)" NICKNAME="Z calibration (dist/px)" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Set manual temporal calibration" NICKNAME="Set manual temporal calibration" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Frame interval (time/frame)" NICKNAME="Frame interval (time/frame)" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Force bit depth" NICKNAME="Force bit depth" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output bit depth" NICKNAME="Output bit depth" VALUE="8" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Minimum input intensity" NICKNAME="Minimum input intensity" VALUE="0.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Maximum input intensity" NICKNAME="Maximum input intensity" VALUE="1.0" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.system.GUISeparator" DISABLEABLE="false" ENABLED="true" ID="1694925848319" NAME="GUI separator" NICKNAME="Detect DNA" NOTES="" SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Show in processing view" NICKNAME="Show basic" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in processing view" NICKNAME="Expanded basic GUI" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in editing view" NICKNAME="Expanded editing GUI" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.images.process.FilterImage" DISABLEABLE="false" ENABLED="true" ID="1694706310794" NAME="Filter image" NICKNAME="Filter image" NOTES="The first processing step is to remove some of the noise in the raw image.  To do this, we apply a 2D Gaussian filter with a sigma of 1px.  This reduces the noise, but retains the DNA features, which are of a similar width to the chosen sigma value.&amp;#10;&amp;#10;The filtered image is added to the workspace with the name &amp;quot;Filtered&amp;quot;." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Image" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Apply to input image" NICKNAME="Apply to input image" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="Filtered" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Filter mode" NICKNAME="Filter mode" VALUE="Gaussian 2D" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Filter radius" NICKNAME="Filter radius" VALUE="1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Filter radius 2" NICKNAME="Filter radius 2" VALUE="3.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Calibrated units" NICKNAME="Calibrated units" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Rolling filter method" NICKNAME="Rolling filter method" VALUE="Average" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Window indices" NICKNAME="Window indices" VALUE="-1-1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Contour contrast" NICKNAME="Contour contrast" VALUE="Dark line" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.script.RunSingleCommand" DISABLEABLE="false" ENABLED="true" ID="1638299323511" NAME="Run single command" NICKNAME="Run single command" NOTES="The mica substrate on which the DNA is deposited gives a variable background that we wish to remove prior to detection of DNA.  To achieve this, we apply rolling ball background subtraction with a ball radius of 5px.  We can use a relatively small radius as we know the DNA shouldn't be wider than approximately 2-3px.&amp;#10;&amp;#10;MIA doesn't have an explicit module to run the rolling ball subtraction.  Instead, we can run this as a single macro command using the &amp;quot;Run single command&amp;quot; module.  This module is compatible with any ImageJ commands which have a corresponding macro command in the form run(&amp;quot;[command]&amp;quot;, &amp;quot;[arguments]&amp;quot;) and which also update the input image.  To find out if a command is compatible, start ImageJ's macro recorder (Plugins &amp;gt; Macros &amp;gt; Record...) and run the operation manually from the ImageJ interface.&amp;#10;&amp;#10;Since we won't need the &amp;quot;Filtered&amp;quot; image in its original form again, we update this image in the workspace with the background-subtracted image.  This helps reduce unnecessary memory usage. " SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Filtered" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Apply to input image" NICKNAME="Apply to input image" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="Filtered" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Command" NICKNAME="Command" VALUE="Subtract Background..." VISIBLE="false"/&gt;&lt;PARAMETER NAME="Parameters" NICKNAME="Parameters" VALUE="rolling=5" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Enable multithreading" NICKNAME="Enable multithreading" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.images.process.threshold.GlobalAutoThreshold" DISABLEABLE="false" ENABLED="true" ID="1695827300950" NAME="Global auto-threshold" NICKNAME="Global auto-threshold" NOTES="The next step is to binarise the image using the &amp;quot;Global auto-threshold&amp;quot; module.  Here, we use the Otsu method and store the output in the workspace with the name &amp;quot;Binary&amp;quot;." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Filtered" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output mode" NICKNAME="Output mode" VALUE="Calculate and apply" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Apply to input image" NICKNAME="Apply to input image" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="Binary" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Algorithm" NICKNAME="Algorithm" VALUE="Otsu" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Threshold multiplier" NICKNAME="Threshold multiplier" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Use lower threshold limit" NICKNAME="Use lower threshold limit" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Lower threshold limit" NICKNAME="Lower threshold limit" VALUE="0.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Binary logic" NICKNAME="Binary logic" VALUE="Black (0) background" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure on objects" NICKNAME="Measure on objects" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" IMAGE_NAME="Binary" NAME="THRESHOLD // GLOBAL Otsu" NICKNAME="THRESHOLD // GLOBAL Otsu"/&gt;&lt;/IMAGE_MEASUREMENTS&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.detect.IdentifyObjects" DISABLEABLE="false" ENABLED="true" ID="1694706262899" NAME="Identify objects" NICKNAME="Identify objects" NOTES="The individual DNA objects are detected from the binary image using connected components labelling.  This process is done using the &amp;quot;Identify objects&amp;quot; module, which takes a binary image and identifies each connected (or 'contiguous') region as a separate object.&amp;#10;&amp;#10;These objects are added to the MIA workspace with the name DNA.&amp;#10;&amp;#10;To perform connected components labelling, MIA uses the MorphoLibJ plugin." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Binary" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output objects" NICKNAME="Output objects" VALUE="DNA" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Binary logic" NICKNAME="Binary logic" VALUE="Black (0) background" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Detection mode" NICKNAME="Detection mode" VALUE="3D" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Identify as single object" NICKNAME="Identify as single object" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Connectivity" NICKNAME="Connectivity" VALUE="26" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Volume type" NICKNAME="Volume type" VALUE="Quadtree" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Enable multithreading" NICKNAME="Enable multithreading" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Minimum strip width (px)" NICKNAME="Minimum strip width (px)" VALUE="60" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.filter.FilterOnImageEdge" DISABLEABLE="false" ENABLED="true" ID="1694706063682" NAME="Remove on image edge" NICKNAME="Remove on image edge" NOTES="One of the aims of this workflow is to measure the length of each single DNA molecule (i.e. not those where multiple molecules are overlapping).  As such, we can't accurately measure any that are in contact with the image edge.  To remove these, we use the &amp;quot;Remove on image edge&amp;quot; module.&amp;#10;&amp;#10;If we were simply counting objects, we may wish to only discard objects touching a couple of image edges (e.g. top and left); however, in this instance we want to remove DNA molecules touching any of the image edges." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="DNA" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Filter mode" NICKNAME="Filter mode" VALUE="Remove filtered objects" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output (filtered) objects" NICKNAME="Output (filtered) objects" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Maximum permitted contact" NICKNAME="Maximum permitted contact" VALUE="0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Remove on top" NICKNAME="Remove on top" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Remove on left" NICKNAME="Remove on left" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Remove on bottom" NICKNAME="Remove on bottom" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Remove on right" NICKNAME="Remove on right" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Include Z-position" NICKNAME="Include Z-position" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Store filter results" NICKNAME="Store filter results" VALUE="false" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.measure.spatial.MeasureObjectShape" DISABLEABLE="false" ENABLED="true" ID="1694998855476" NAME="Measure object shape" NICKNAME="Measure object shape" NOTES="At the moment, the &amp;quot;DNA&amp;quot; object collection contains a lot of small round objects which likely correspond to salt crystals and other debris.  To remove these, we can set a minimum diameter.&amp;#10;&amp;#10;First, we make this measurement using the &amp;quot;Measure object shape&amp;quot; module.  Measurements in 2D are calculated on Z-projected objects; however, as our objects are in 2D already this will make no difference." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="DNA" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure volume" NICKNAME="Measure volume" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure projected area" NICKNAME="Measure projected area" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure projected diameter" NICKNAME="Measure projected diameter" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure projected perimeter" NICKNAME="Measure projected perimeter" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measure 3D metrics" NICKNAME="Measure 3D metrics" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Connectivity" NICKNAME="Connectivity" VALUE="26" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Surface area method" NICKNAME="Surface area method" VALUE="13 directions" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Enable multithreading" NICKNAME="Enable multithreading" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SHAPE // PROJ_DIA_(PX)" NICKNAME="SHAPE // PROJ_DIA_(PX)" OBJECT_NAME="DNA"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SHAPE // PROJ_DIA_(µm)" NICKNAME="SHAPE // PROJ_DIA_(µm)" OBJECT_NAME="DNA"/&gt;&lt;/OBJECT_MEASUREMENTS&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.filter.FilterByMeasurement" DISABLEABLE="true" ENABLED="true" ID="1694998908258" NAME="Based on measurement" NICKNAME="Based on measurement" NOTES="With the diameter measurements calculated, we can remove any &amp;quot;DNA&amp;quot; objects smaller than a specific size using the &amp;quot;Based on measurement&amp;quot; filter module." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="DNA" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Filter mode" NICKNAME="Filter mode" VALUE="Remove filtered objects" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output (filtered) objects" NICKNAME="Output (filtered) objects" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Method for filtering" NICKNAME="Method for filtering" VALUE="Less than" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference mode" NICKNAME="Reference mode" VALUE="Fixed value" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference value" NICKNAME="Reference value" VALUE="20" VISIBLE="true"/&gt;&lt;PARAMETER NAME="Reference value image" NICKNAME="Reference value image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference image measurement" NICKNAME="Reference image measurement" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference value parent object" NICKNAME="Reference value parent object" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference object measurement" NICKNAME="Reference object measurement" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference value multiplier" NICKNAME="Reference value multiplier" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Store summary filter results" NICKNAME="Store summary filter results" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Store individual filter results" NICKNAME="Store individual filter results" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measurement to filter on" NICKNAME="Measurement to filter on" VALUE="SHAPE // PROJ_DIA_(PX)" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.system.GUISeparator" DISABLEABLE="false" ENABLED="true" ID="1694925858241" NAME="GUI separator" NICKNAME="Measurements" NOTES="" SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Show in processing view" NICKNAME="Show basic" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in processing view" NICKNAME="Expanded basic GUI" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in editing view" NICKNAME="Expanded editing GUI" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.process.CreateSkeleton" DISABLEABLE="false" ENABLED="true" ID="1694925436767" NAME="Create skeleton" NICKNAME="Create skeleton" NOTES="To measure length of our &amp;quot;DNA&amp;quot; objects, we can use the &amp;quot;Measure skeleton&amp;quot; module.  Skeletonisation involves reducing objects to a single pixel-wide line.  During this process, the length of the skeleton objects is measured and added to the associated DNA object.&amp;#10;&amp;#10;Skeletons themselves are formed from networks of &amp;quot;Edges&amp;quot; and &amp;quot;Junctions&amp;quot;, where edges are line segments between two junctions.  Junctions can in turn have one or more connected edges.&amp;#10;&amp;#10;MIA provides two object relationship types, both of which are in use when creating skeletons.  Parent-child relationships allow for one-to-many relationships between objects and here, the &amp;quot;DNA&amp;quot; objects are parents to the child &amp;quot;Skeleton&amp;quot; objects.  Likewise, the &amp;quot;Edges&amp;quot; and &amp;quot;Junctions&amp;quot; are children of the &amp;quot;Skeleton&amp;quot; objects.  Since MIA allows for extended relationships, this means the &amp;quot;Edges&amp;quot; and &amp;quot;Junctions&amp;quot; are therefore grandchildren of the &amp;quot;DNA&amp;quot; objects.&amp;#10;&amp;#10;Conversely, partner relationships allow for many-to-many relationships and here are present between &amp;quot;Edges&amp;quot; and &amp;quot;Junctions&amp;quot;.&amp;#10;&amp;#10;The &amp;quot;Measure skeleton&amp;quot; module  uses the &amp;quot;Analyze Skeleton&amp;quot; ImageJ plugin." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.1.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input mode" NICKNAME="Input mode" VALUE="Objects" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Binary logic" NICKNAME="Binary logic" VALUE="Black (0) background" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="DNA" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Add skeletons to workspace" NICKNAME="Add skeletons to workspace" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output skeleton objects" NICKNAME="Output skeleton objects" VALUE="Skeletons" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output edge objects" NICKNAME="Output edge objects" VALUE="Edges" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output junction objects" NICKNAME="Output junction objects" VALUE="Junctions" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Export loop objects" NICKNAME="Export loop objects" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output loop objects" NICKNAME="Output loop objects" VALUE="Loops" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Export largest shortest path" NICKNAME="Export largest shortest path" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output largest shortest path" NICKNAME="Output largest shortest path" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Minimum branch length" NICKNAME="Minimum branch length" VALUE="5" VISIBLE="true"/&gt;&lt;PARAMETER NAME="Calibrated units" NICKNAME="Calibrated units" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Enable multithreading" NICKNAME="Enable multithreading" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SKELETON // LENGTH_(PX)" NICKNAME="SKELETON // LENGTH_(PX)" OBJECT_NAME="Edges"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" EXPORT_MAX="false" EXPORT_MEAN="true" EXPORT_MIN="false" EXPORT_STD="true" EXPORT_SUM="true" NAME="SKELETON // LENGTH_(µm)" NICKNAME="SKELETON // LENGTH_(µm)" OBJECT_NAME="Edges"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SKELETON // SUM_LENGTH_(PX)" NICKNAME="SKELETON // SUM_LENGTH_(PX)" OBJECT_NAME="DNA"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" EXPORT_MAX="false" EXPORT_MEAN="true" EXPORT_MIN="false" EXPORT_STD="true" EXPORT_SUM="true" NAME="SKELETON // SUM_LENGTH_(µm)" NICKNAME="SKELETON // SUM_LENGTH_(µm)" OBJECT_NAME="DNA"/&gt;&lt;/OBJECT_MEASUREMENTS&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.filter.FilterByPartners" DISABLEABLE="false" ENABLED="true" ID="1694706692780" NAME="Number of partners" NICKNAME="Number of partners" NOTES="For our analysis, we only want to measure the length of individual DNA molecules.  That means, we need a way of identifying any &amp;quot;DNA&amp;quot; objects formed from multiple overlapping molecules.&amp;#10;&amp;#10;One way to do this is to count the number of lose DNA ends there are, which we can do by counting the number of &amp;quot;Junction&amp;quot; objects which only have a single connected &amp;quot;Edge&amp;quot;.  For this, we use the &amp;quot;Number of partners&amp;quot; object filter.  With this filter we don't want to remove any junctions with a single connected edge; rather, we want to move them to a separate class which we call &amp;quot;Ends&amp;quot;.&amp;#10;&amp;#10;The &amp;quot;Ends&amp;quot; objects are added to the MIA workspace and automatically inherit any relationships that same object had when it was a &amp;quot;Junction&amp;quot;.  In this case these are direct relationships with &amp;quot;Skeleton&amp;quot; and &amp;quot;Edge&amp;quot; objects as well as the extended grandparent-grandchild relationship to &amp;quot;DNA&amp;quot; that arises as a result of being a child of an object (&amp;quot;Skeletons&amp;quot;) which itself is a child of a &amp;quot;DNA&amp;quot; object." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="Junctions" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Filter mode" NICKNAME="Filter mode" VALUE="Move filtered objects to new class" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output (filte</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>red) objects" NICKNAME="Output (filtered) objects" VALUE="Ends" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Method for filtering" NICKNAME="Method for filtering" VALUE="Equal to" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference mode" NICKNAME="Reference mode" VALUE="Fixed value" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference value" NICKNAME="Reference value" VALUE="1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference value image" NICKNAME="Reference value image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference image measurement" NICKNAME="Reference image measurement" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference value parent object" NICKNAME="Reference value parent object" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference object measurement" NICKNAME="Reference object measurement" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference value multiplier" NICKNAME="Reference value multiplier" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Store summary filter results" NICKNAME="Store summary filter results" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Store individual filter results" NICKNAME="Store individual filter results" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Partner objects" NICKNAME="Partner objects" VALUE="Edges" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.filter.FilterByChildren" DISABLEABLE="false" ENABLED="true" ID="1694706728197" NAME="Number of children" NICKNAME="Number of children" NOTES="We can now estimate which &amp;quot;DNA&amp;quot; objects are formed from multiple overlapping DNA molecules based on the number of grandchild &amp;quot;Enda&amp;quot; object relationships they have. &amp;#10;&amp;#10;Using the &amp;quot;Number of children&amp;quot; module, we can apply this filter and move any &amp;quot;DNA&amp;quot; objectw with more than 2 &amp;quot;Ends&amp;quot; grandchildren to a new object collection called &amp;quot;Networks&amp;quot;. As before, the objects moved to the new collection will retain all existing relationships and measurements, meaning we can export the length of each &amp;quot;Network&amp;quot; object." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="DNA" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Filter mode" NICKNAME="Filter mode" VALUE="Move filtered objects to new class" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output (filtered) objects" NICKNAME="Output (filtered) objects" VALUE="Networks" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Method for filtering" NICKNAME="Method for filtering" VALUE="Greater than" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference mode" NICKNAME="Reference mode" VALUE="Fixed value" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference value" NICKNAME="Reference value" VALUE="2" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference value image" NICKNAME="Reference value image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference image measurement" NICKNAME="Reference image measurement" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference value parent object" NICKNAME="Reference value parent object" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference object measurement" NICKNAME="Reference object measurement" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference value multiplier" NICKNAME="Reference value multiplier" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Store summary filter results" NICKNAME="Store summary filter results" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Store individual filter results" NICKNAME="Store individual filter results" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Child objects" NICKNAME="Child objects" VALUE="Skeletons // Ends" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SHAPE // PROJ_DIA_(PX)" NICKNAME="SHAPE // PROJ_DIA_(PX)" OBJECT_NAME="Networks"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SHAPE // PROJ_DIA_(µm)" NICKNAME="SHAPE // PROJ_DIA_(µm)" OBJECT_NAME="Networks"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SKELETON // SUM_LENGTH_(PX)" NICKNAME="SKELETON // SUM_LENGTH_(PX)" OBJECT_NAME="Networks"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" EXPORT_MAX="false" EXPORT_MEAN="true" EXPORT_MIN="false" EXPORT_STD="true" EXPORT_SUM="true" NAME="SKELETON // SUM_LENGTH_(µm)" NICKNAME="SKELETON // SUM_LENGTH_(µm)" OBJECT_NAME="Networks"/&gt;&lt;/OBJECT_MEASUREMENTS&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.measure.miscellaneous.ParentObjectID" DISABLEABLE="false" ENABLED="true" ID="1696040403713" NAME="Parent object ID" NICKNAME="Parent object ID" NOTES="The &amp;quot;Parent object ID&amp;quot; module adds a measurement to the selected object, containing the ID (if any) of a particular parent class. This can be exported to the Excel spreadsheet. &amp;#10;&amp;#10;Here, for the &amp;quot;Edges&amp;quot; objects, we're adding the ID of the grandparent &amp;quot;DNA&amp;quot; object." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="Edges" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Parent object" NICKNAME="Parent object" VALUE="Skeletons // DNA" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS&gt;&lt;MEASUREMENT EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" EXPORT_MAX="false" EXPORT_MEAN="false" EXPORT_MIN="false" EXPORT_STD="false" EXPORT_SUM="false" NAME="PARENT_ID // Skeletons // DNA" NICKNAME="PARENT_ID // Skeletons // DNA" OBJECT_NAME="Edges"/&gt;&lt;/OBJECT_MEASUREMENTS&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.measure.miscellaneous.ParentObjectID" DISABLEABLE="false" ENABLED="true" ID="1696460149571" NAME="Parent object ID" NICKNAME="Parent object ID" NOTES="As with the previous module, we're adding a measurement that reports the ID number of the grandparent &amp;quot;Network&amp;quot; ovjects." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="Edges" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Parent object" NICKNAME="Parent object" VALUE="Skeletons // Networks" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS&gt;&lt;MEASUREMENT EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" EXPORT_MAX="false" EXPORT_MEAN="false" EXPORT_MIN="false" EXPORT_STD="false" EXPORT_SUM="false" NAME="PARENT_ID // Skeletons // Networks" NICKNAME="PARENT_ID // Skeletons // Networks" OBJECT_NAME="Edges"/&gt;&lt;/OBJECT_MEASUREMENTS&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.system.GUISeparator" DISABLEABLE="false" ENABLED="true" ID="1694925755615" NAME="GUI separator" NICKNAME="Image output" NOTES="" SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Show in processing view" NICKNAME="Show basic" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in processing view" NICKNAME="Expanded basic GUI" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in editing view" NICKNAME="Expanded editing GUI" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.images.configure.SetDisplayRange" DISABLEABLE="false" ENABLED="true" ID="1694926127961" NAME="Set intensity display range" NICKNAME="Set intensity display range" NOTES="For the purpose of visualisation, the &amp;quot;Filtered&amp;quot; image is used. To make the DNA molecules easier to see, the intensity display range of the image is adjusted. This process doesnr affect the pixel information stored in the image, rather it chamges how the image is displayed on screen. &amp;#10;&amp;#10;The &amp;quot;precise&amp;quot; method hwre allows us to specify the fraction of pixels that will have clipped intensities at the top and bottom of the display range. &amp;#10;&amp;#10;This module adds a new &amp;quot;Overlay&amp;quot; image to the workspace. " SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Filtered" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Apply to input image" NICKNAME="Apply to input image" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="Overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Calculation mode" NICKNAME="Calculation mode" VALUE="Precise" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Calculation source" NICKNAME="Calculation source" VALUE="Internal" VISIBLE="false"/&gt;&lt;PARAMETER NAME="External source" NICKNAME="External source" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Clipping fraction (min)" NICKNAME="Clipping fraction (min)" VALUE="0.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Clipping fraction (max)" NICKNAME="Clipping fraction (max)" VALUE="0.01" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Set minimum value" NICKNAME="Set minimum value" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Set maximum value" NICKNAME="Set maximum value" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Minimum range value" NICKNAME="Minimum range value" VALUE="0.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Maximum range value" NICKNAME="Maximum range value" VALUE="255.0" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.visualise.overlays.AddObjectFill" DISABLEABLE="false" ENABLED="true" ID="1694705240541" NAME="Add object fill" NICKNAME="Add object fill" NOTES="In this example we'll display the DNA as a fill overlay, rather than an outline. a fill is an overlay thst goes over the top of the entire pixel. &amp;#10;&amp;#10;In order to see some of the pixel intensity, the opacity has been set to 50%. All single DNA molecules detected by this workflow are coloured cyan - this will contrast the overlapping molecules stored in the &amp;quot;Networks&amp;quot; collection, which we'll colour magenta in the next step." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Colour mode" NICKNAME="Colour mode" VALUE="Single colour" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Colour map" NICKNAME="Colour map" VALUE="Spectrum" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Single colour" NICKNAME="Single colour" VALUE="Cyan" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Child objects for colour" NICKNAME="Child objects for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measurement for colour" NICKNAME="Measurement for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Parent object for colour" NICKNAME="Parent object for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Partner objects for colour" NICKNAME="Partner objects for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Opacity (%)" NICKNAME="Opacity (%)" VALUE="100" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Range minimum mode" NICKNAME="Range minimum mode" VALUE="Automatic" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Minimum value" NICKNAME="Minimum value" VALUE="0.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Range maximum mode" NICKNAME="Range maximum mode" VALUE="Automatic" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Maximum value" NICKNAME="Maximum value" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="DNA" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Apply to input image" NICKNAME="Apply to input image" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Add output image to workspace" NICKNAME="Add output image to workspace" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="Overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Render in all frames" NICKNAME="Render in all frames" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Enable multithreading" NICKNAME="Enable multithreading" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.visualise.overlays.AddObjectFill" DISABLEABLE="false" ENABLED="true" ID="1694706046687" NAME="Add object fill" NICKNAME="Add object fill" NOTES="As with the &amp;quot;DNA&amp;quot; objects, we render the &amp;quot;Networks&amp;quot; objects with a fill overlay. The only difference ia that they're coloured magenta." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Colour mode" NICKNAME="Colour mode" VALUE="Single colour" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Colour map" NICKNAME="Colour map" VALUE="Spectrum" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Single colour" NICKNAME="Single colour" VALUE="Magenta" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Child objects for colour" NICKNAME="Child objects for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measurement for colour" NICKNAME="Measurement for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Parent object for colour" NICKNAME="Parent object for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Partner objects for colour" NICKNAME="Partner objects for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Opacity (%)" NICKNAME="Opacity (%)" VALUE="100.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Range minimum mode" NICKNAME="Range minimum mode" VALUE="Automatic" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Minimum value" NICKNAME="Minimum value" VALUE="0.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Range maximum mode" NICKNAME="Range maximum mode" VALUE="Automatic" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Maximum value" NICKNAME="Maximum value" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="Networks" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Apply to input image" NICKNAME="Apply to input image" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Add output image to workspace" NICKNAME="Add output image to workspace" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="Overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Render in all frames" NICKNAME="Render in all frames" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Enable multithreading" NICKNAME="Enable multithreading" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.visualise.ShowImage" DISABLEABLE="true" ENABLED="true" ID="1694925777350" NAME="Show image" NICKNAME="Show image" NOTES="Optionally displaying the image." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="true" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Display image" NICKNAME="Display image" VALUE="Overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Title mode" NICKNAME="Title mode" VALUE="Image name" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Quick normalisation" NICKNAME="Quick normalisation" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Channel mode" NICKNAME="Channel mode" VALUE="Composite" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.inputoutput.ImageSaver" DISABLEABLE="true" ENABLED="true" ID="1694925777350" NAME="Save image" NICKNAME="Save image" NOTES="Optionally saving the image to the same folder as the input image, but woth the suffix &amp;quot;_overlay&amp;quot;." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Save location" NICKNAME="Save location" VALUE="Save with input file" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Mirrored directory root" NICKNAME="Mirrored directory root" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File path" NICKNAME="File path" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File name (generic)" NICKNAME="File name (generic)" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Save name mode" NICKNAME="Save name mode" VALUE="Match input file name" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File name" NICKNAME="File name" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Append series mode" NICKNAME="Append series mode" VALUE="None" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Append date/time mode" NICKNAME="Append date/time mode" VALUE="Never" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Add filename suffix" NICKNAME="Add filename suffix" VALUE="_overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File format" NICKNAME="File format" VALUE="TIF" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Channel mode" NICKNAME="Channel mode" VALUE="Composite" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Save as RGB" NICKNAME="Save as RGB" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Compression mode" NICKNAME="Compression mode" VALUE="None" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Quality (0-100)" NICKNAME="Quality (0-100)" VALUE="100" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Frame rate (fps)" NICKNAME="Frame rate (fps)" VALUE="25" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Flatten overlay" NICKNAME="Flatten overlay" VALUE="false" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;/MODULES&gt;&lt;/ROOT&gt;</t>
+          <t>METER NAME="Output (filtered) objects" NICKNAME="Output (filtered) objects" VALUE="Ends" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Method for filtering" NICKNAME="Method for filtering" VALUE="Equal to" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference mode" NICKNAME="Reference mode" VALUE="Fixed value" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference value" NICKNAME="Reference value" VALUE="1" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference value image" NICKNAME="Reference value image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference image measurement" NICKNAME="Reference image measurement" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference value parent object" NICKNAME="Reference value parent object" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference object measurement" NICKNAME="Reference object measurement" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference value multiplier" NICKNAME="Reference value multiplier" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Store summary filter results" NICKNAME="Store summary filter results" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Store individual filter results" NICKNAME="Store individual filter results" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Partner objects" NICKNAME="Partner objects" VALUE="Edges" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.filter.FilterByChildren" DISABLEABLE="false" ENABLED="true" ID="1694706728197" NAME="Number of children" NICKNAME="Number of children" NOTES="We can now estimate which &amp;quot;DNA&amp;quot; objects are formed from multiple overlapping DNA molecules based on the number of grandchild &amp;quot;Enda&amp;quot; object relationships they have. &amp;#10;&amp;#10;Using the &amp;quot;Number of children&amp;quot; module, we can apply this filter and move any &amp;quot;DNA&amp;quot; objectw with more than 2 &amp;quot;Ends&amp;quot; grandchildren to a new object collection called &amp;quot;Networks&amp;quot;. As before, the objects moved to the new collection will retain all existing relationships and measurements, meaning we can export the length of each &amp;quot;Network&amp;quot; object." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="DNA" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Filter mode" NICKNAME="Filter mode" VALUE="Move filtered objects to new class" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output (filtered) objects" NICKNAME="Output (filtered) objects" VALUE="Networks" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Method for filtering" NICKNAME="Method for filtering" VALUE="Greater than" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference mode" NICKNAME="Reference mode" VALUE="Fixed value" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference value" NICKNAME="Reference value" VALUE="2" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference value image" NICKNAME="Reference value image" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference image measurement" NICKNAME="Reference image measurement" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference value parent object" NICKNAME="Reference value parent object" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference object measurement" NICKNAME="Reference object measurement" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Reference value multiplier" NICKNAME="Reference value multiplier" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Store summary filter results" NICKNAME="Store summary filter results" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Store individual filter results" NICKNAME="Store individual filter results" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Child objects" NICKNAME="Child objects" VALUE="Skeletons // Ends" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SHAPE // PROJ_DIA_(PX)" NICKNAME="SHAPE // PROJ_DIA_(PX)" OBJECT_NAME="Networks"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SHAPE // PROJ_DIA_(µm)" NICKNAME="SHAPE // PROJ_DIA_(µm)" OBJECT_NAME="Networks"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="false" EXPORT_INDIVIDUAL="true" EXPORT_MAX="true" EXPORT_MEAN="true" EXPORT_MIN="true" EXPORT_STD="true" EXPORT_SUM="true" NAME="SKELETON // SUM_LENGTH_(PX)" NICKNAME="SKELETON // SUM_LENGTH_(PX)" OBJECT_NAME="Networks"/&gt;&lt;MEASUREMENT EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" EXPORT_MAX="false" EXPORT_MEAN="true" EXPORT_MIN="false" EXPORT_STD="true" EXPORT_SUM="true" NAME="SKELETON // SUM_LENGTH_(µm)" NICKNAME="SKELETON // SUM_LENGTH_(µm)" OBJECT_NAME="Networks"/&gt;&lt;/OBJECT_MEASUREMENTS&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.measure.miscellaneous.ParentObjectID" DISABLEABLE="false" ENABLED="true" ID="1696040403713" NAME="Parent object ID" NICKNAME="Parent object ID" NOTES="The &amp;quot;Parent object ID&amp;quot; module adds a measurement to the selected object, containing the ID (if any) of a particular parent class. This can be exported to the Excel spreadsheet. &amp;#10;&amp;#10;Here, for the &amp;quot;Edges&amp;quot; objects, we're adding the ID of the grandparent &amp;quot;DNA&amp;quot; object." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="Edges" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Parent object" NICKNAME="Parent object" VALUE="Skeletons // DNA" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS&gt;&lt;MEASUREMENT EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" EXPORT_MAX="false" EXPORT_MEAN="false" EXPORT_MIN="false" EXPORT_STD="false" EXPORT_SUM="false" NAME="PARENT_ID // Skeletons // DNA" NICKNAME="PARENT_ID // Skeletons // DNA" OBJECT_NAME="Edges"/&gt;&lt;/OBJECT_MEASUREMENTS&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.objects.measure.miscellaneous.ParentObjectID" DISABLEABLE="false" ENABLED="true" ID="1696460149571" NAME="Parent object ID" NICKNAME="Parent object ID" NOTES="As with the previous module, we're adding a measurement that reports the ID number of the grandparent &amp;quot;Network&amp;quot; ovjects." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="Edges" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Parent object" NICKNAME="Parent object" VALUE="Skeletons // Networks" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS&gt;&lt;MEASUREMENT EXPORT_GLOBAL="true" EXPORT_INDIVIDUAL="true" EXPORT_MAX="false" EXPORT_MEAN="false" EXPORT_MIN="false" EXPORT_STD="false" EXPORT_SUM="false" NAME="PARENT_ID // Skeletons // Networks" NICKNAME="PARENT_ID // Skeletons // Networks" OBJECT_NAME="Edges"/&gt;&lt;/OBJECT_MEASUREMENTS&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.system.GUISeparator" DISABLEABLE="false" ENABLED="true" ID="1694925755615" NAME="GUI separator" NICKNAME="Image output" NOTES="" SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Show in processing view" NICKNAME="Show basic" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in processing view" NICKNAME="Expanded basic GUI" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Expanded in editing view" NICKNAME="Expanded editing GUI" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.images.configure.SetDisplayRange" DISABLEABLE="false" ENABLED="true" ID="1694926127961" NAME="Set intensity display range" NICKNAME="Set intensity display range" NOTES="For the purpose of visualisation, the &amp;quot;Filtered&amp;quot; image is used. To make the DNA molecules easier to see, the intensity display range of the image is adjusted. This process doesnr affect the pixel information stored in the image, rather it chamges how the image is displayed on screen. &amp;#10;&amp;#10;The &amp;quot;precise&amp;quot; method hwre allows us to specify the fraction of pixels that will have clipped intensities at the top and bottom of the display range. &amp;#10;&amp;#10;This module adds a new &amp;quot;Overlay&amp;quot; image to the workspace. " SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.1"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Filtered" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Apply to input image" NICKNAME="Apply to input image" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="Overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Calculation mode" NICKNAME="Calculation mode" VALUE="Precise" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Calculation source" NICKNAME="Calculation source" VALUE="Internal" VISIBLE="false"/&gt;&lt;PARAMETER NAME="External source" NICKNAME="External source" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Clipping fraction (min)" NICKNAME="Clipping fraction (min)" VALUE="0.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Clipping fraction (max)" NICKNAME="Clipping fraction (max)" VALUE="0.01" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Set minimum value" NICKNAME="Set minimum value" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Set maximum value" NICKNAME="Set maximum value" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Minimum range value" NICKNAME="Minimum range value" VALUE="0.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Maximum range value" NICKNAME="Maximum range value" VALUE="255.0" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.visualise.overlays.AddObjectFill" DISABLEABLE="false" ENABLED="true" ID="1694705240541" NAME="Add object fill" NICKNAME="Add object fill" NOTES="In this example we'll display the DNA as a fill overlay, rather than an outline. a fill is an overlay thst goes over the top of the entire pixel. &amp;#10;&amp;#10;In order to see some of the pixel intensity, the opacity has been set to 50%. All single DNA molecules detected by this workflow are coloured cyan - this will contrast the overlapping molecules stored in the &amp;quot;Networks&amp;quot; collection, which we'll colour magenta in the next step." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Colour mode" NICKNAME="Colour mode" VALUE="Single colour" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Colour map" NICKNAME="Colour map" VALUE="Spectrum" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Single colour" NICKNAME="Single colour" VALUE="Cyan" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Child objects for colour" NICKNAME="Child objects for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measurement for colour" NICKNAME="Measurement for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Parent object for colour" NICKNAME="Parent object for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Partner objects for colour" NICKNAME="Partner objects for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Opacity (%)" NICKNAME="Opacity (%)" VALUE="100" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Range minimum mode" NICKNAME="Range minimum mode" VALUE="Automatic" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Minimum value" NICKNAME="Minimum value" VALUE="0.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Range maximum mode" NICKNAME="Range maximum mode" VALUE="Automatic" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Maximum value" NICKNAME="Maximum value" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="DNA" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Apply to input image" NICKNAME="Apply to input image" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Add output image to workspace" NICKNAME="Add output image to workspace" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="Overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Render in all frames" NICKNAME="Render in all frames" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Enable multithreading" NICKNAME="Enable multithreading" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.visualise.overlays.AddObjectFill" DISABLEABLE="false" ENABLED="true" ID="1694706046687" NAME="Add object fill" NICKNAME="Add object fill" NOTES="As with the &amp;quot;DNA&amp;quot; objects, we render the &amp;quot;Networks&amp;quot; objects with a fill overlay. The only difference ia that they're coloured magenta." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Colour mode" NICKNAME="Colour mode" VALUE="Single colour" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Colour map" NICKNAME="Colour map" VALUE="Spectrum" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Single colour" NICKNAME="Single colour" VALUE="Magenta" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Child objects for colour" NICKNAME="Child objects for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Measurement for colour" NICKNAME="Measurement for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Parent object for colour" NICKNAME="Parent object for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Partner objects for colour" NICKNAME="Partner objects for colour" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Opacity (%)" NICKNAME="Opacity (%)" VALUE="100.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Range minimum mode" NICKNAME="Range minimum mode" VALUE="Automatic" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Minimum value" NICKNAME="Minimum value" VALUE="0.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Range maximum mode" NICKNAME="Range maximum mode" VALUE="Automatic" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Maximum value" NICKNAME="Maximum value" VALUE="1.0" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input objects" NICKNAME="Input objects" VALUE="Networks" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Apply to input image" NICKNAME="Apply to input image" VALUE="true" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Add output image to workspace" NICKNAME="Add output image to workspace" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Output image" NICKNAME="Output image" VALUE="Overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Render in all frames" NICKNAME="Render in all frames" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Enable multithreading" NICKNAME="Enable multithreading" VALUE="true" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.visualise.ShowImage" DISABLEABLE="true" ENABLED="true" ID="1694925777350" NAME="Show image" NICKNAME="Show image" NOTES="Optionally displaying the image." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="true" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Display image" NICKNAME="Display image" VALUE="Overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Title mode" NICKNAME="Title mode" VALUE="Image name" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Quick normalisation" NICKNAME="Quick normalisation" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Channel mode" NICKNAME="Channel mode" VALUE="Composite" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;MODULE CLASSNAME="io.github.mianalysis.mia.module.inputoutput.ImageSaver" DISABLEABLE="true" ENABLED="true" ID="1694925777350" NAME="Save image" NICKNAME="Save image" NOTES="Optionally saving the image to the same folder as the input image, but woth the suffix &amp;quot;_overlay&amp;quot;." SHOW_BASIC_TITLE="true" SHOW_OUTPUT="false" VERSION="1.0.0"&gt;&lt;PARAMETERS&gt;&lt;PARAMETER NAME="Save location" NICKNAME="Save location" VALUE="Save with input file" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Mirrored directory root" NICKNAME="Mirrored directory root" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File path" NICKNAME="File path" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File name (generic)" NICKNAME="File name (generic)" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Save name mode" NICKNAME="Save name mode" VALUE="Match input file name" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File name" NICKNAME="File name" VALUE="" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Append series mode" NICKNAME="Append series mode" VALUE="None" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Append date/time mode" NICKNAME="Append date/time mode" VALUE="Never" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Add filename suffix" NICKNAME="Add filename suffix" VALUE="_overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Input image" NICKNAME="Input image" VALUE="Overlay" VISIBLE="false"/&gt;&lt;PARAMETER NAME="File format" NICKNAME="File format" VALUE="TIF" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Channel mode" NICKNAME="Channel mode" VALUE="Composite" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Save as RGB" NICKNAME="Save as RGB" VALUE="false" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Compression mode" NICKNAME="Compression mode" VALUE="None" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Quality (0-100)" NICKNAME="Quality (0-100)" VALUE="100" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Frame rate (fps)" NICKNAME="Frame rate (fps)" VALUE="25" VISIBLE="false"/&gt;&lt;PARAMETER NAME="Flatten overlay" NICKNAME="Flatten overlay" VALUE="false" VISIBLE="false"/&gt;&lt;/PARAMETERS&gt;&lt;IMAGE_MEASUREMENTS/&gt;&lt;OBJECT_MEASUREMENTS/&gt;&lt;METADATA/&gt;&lt;/MODULE&gt;&lt;/MODULES&gt;&lt;/ROOT&gt;</t>
         </is>
       </c>
     </row>
@@ -5352,7 +5352,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5361,7 +5361,18 @@
     <row r="1">
       <c r="A1" s="17" t="inlineStr">
         <is>
-          <t>LOG</t>
+          <t>ERROR LOG</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+</row>
+    <row r="3">
+</row>
+    <row r="4">
+      <c r="A4" s="17" t="inlineStr">
+        <is>
+          <t>WARNING LOG</t>
         </is>
       </c>
     </row>

</xml_diff>